<commit_message>
update XLS for pgns
</commit_message>
<xml_diff>
--- a/Support/PGN 5.6.xlsx
+++ b/Support/PGN 5.6.xlsx
@@ -10,7 +10,7 @@
     <sheet name="PGN" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">PGN!$B$1:$Q$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PGN!$A$1:$Q$66</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="171">
   <si>
     <t>Src</t>
   </si>
@@ -520,13 +520,34 @@
   </si>
   <si>
     <t>Port = 5126</t>
+  </si>
+  <si>
+    <t>123,  7B</t>
+  </si>
+  <si>
+    <t>126,  7E</t>
+  </si>
+  <si>
+    <t>121, 79</t>
+  </si>
+  <si>
+    <t>124,  7C</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>IP,  MAC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +600,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -598,7 +633,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -819,12 +854,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -833,7 +892,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1058,13 +1117,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1386,11 +1457,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AG60"/>
+  <dimension ref="B1:AG65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1763,7 +1834,10 @@
       <c r="T12" s="25"/>
       <c r="U12" s="25"/>
     </row>
-    <row r="13" spans="2:24" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:24" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="C13" s="62"/>
       <c r="D13" s="71"/>
       <c r="E13" s="57"/>
@@ -1784,10 +1858,7 @@
       <c r="T13" s="22"/>
       <c r="U13" s="22"/>
     </row>
-    <row r="14" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>137</v>
-      </c>
+    <row r="14" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="62" t="s">
         <v>126</v>
       </c>
@@ -1835,9 +1906,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B15" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
     <row r="16" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>127</v>
@@ -1888,12 +1964,12 @@
     </row>
     <row r="17" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
-        <v>154</v>
+      <c r="B18" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="C18" s="62" t="s">
         <v>120</v>
@@ -1990,11 +2066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
+    <row r="19" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="62" t="s">
         <v>77</v>
@@ -2030,7 +2102,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>59</v>
+      </c>
       <c r="C22" s="64"/>
       <c r="D22" s="73"/>
       <c r="E22" s="59"/>
@@ -2051,11 +2126,9 @@
       <c r="T22" s="27"/>
       <c r="U22" s="27"/>
     </row>
-    <row r="23" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="83" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="82" t="s">
+    <row r="23" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="11"/>
+      <c r="C23" s="62" t="s">
         <v>145</v>
       </c>
       <c r="D23" s="71">
@@ -2101,7 +2174,9 @@
       <c r="U23" s="22"/>
     </row>
     <row r="24" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="11"/>
+      <c r="B24" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="C24" s="62"/>
       <c r="D24" s="71"/>
       <c r="E24" s="51"/>
@@ -2123,8 +2198,8 @@
       <c r="U24" s="22"/>
     </row>
     <row r="25" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
-        <v>150</v>
+      <c r="B25" s="11" t="s">
+        <v>160</v>
       </c>
       <c r="C25" s="62"/>
       <c r="D25" s="71"/>
@@ -2148,7 +2223,7 @@
     </row>
     <row r="26" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C26" s="62"/>
       <c r="D26" s="71"/>
@@ -2172,7 +2247,7 @@
     </row>
     <row r="27" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C27" s="62"/>
       <c r="D27" s="71"/>
@@ -2195,106 +2270,106 @@
       <c r="U27" s="22"/>
     </row>
     <row r="28" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="B28" s="11"/>
       <c r="C28" s="62"/>
       <c r="D28" s="71"/>
       <c r="E28" s="51"/>
       <c r="F28" s="52"/>
       <c r="G28" s="53"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
-    </row>
-    <row r="29" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="11"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
-      <c r="U29" s="22"/>
-    </row>
-    <row r="30" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="30"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-    </row>
-    <row r="31" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="83" t="s">
+      <c r="H28" s="22"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
+    </row>
+    <row r="29" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="82" t="s">
+      <c r="C29" s="30"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="61"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+    </row>
+    <row r="30" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="D31" s="71" t="s">
+      <c r="D30" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="57">
+      <c r="E30" s="57">
         <v>124</v>
       </c>
-      <c r="F31" s="52" t="s">
+      <c r="F30" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="58">
+      <c r="G30" s="58">
         <v>214</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>113</v>
       </c>
     </row>
+    <row r="31" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
     <row r="32" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="84"/>
-      <c r="C32" s="82"/>
-    </row>
-    <row r="33" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="8" t="s">
-        <v>142</v>
-      </c>
+      <c r="B32" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="31"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="58"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
     </row>
     <row r="34" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="C34" s="31"/>
       <c r="D34" s="71"/>
@@ -2316,15 +2391,13 @@
       <c r="U34" s="22"/>
     </row>
     <row r="35" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C35" s="31"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="71"/>
       <c r="E35" s="57"/>
       <c r="F35" s="52"/>
       <c r="G35" s="58"/>
-      <c r="I35" s="31"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="2"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
       <c r="L35" s="22"/>
@@ -2338,380 +2411,391 @@
       <c r="T35" s="22"/>
       <c r="U35" s="22"/>
     </row>
-    <row r="36" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="58"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="24"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="24"/>
-      <c r="U36" s="24"/>
-    </row>
-    <row r="37" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="62"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-      <c r="T37" s="22"/>
-      <c r="U37" s="22"/>
-    </row>
-    <row r="38" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
+    <row r="36" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="61"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="27"/>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="27"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="61"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="27"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="27"/>
+      <c r="U36" s="27"/>
+    </row>
+    <row r="37" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="57">
+        <v>125</v>
+      </c>
+      <c r="F37" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" s="58">
+        <v>215</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="8" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="39" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" s="71" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" s="57">
-        <v>125</v>
-      </c>
-      <c r="F39" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="G39" s="58">
-        <v>215</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>112</v>
+      <c r="B39" s="11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="8" t="s">
-        <v>139</v>
+      <c r="B40" s="11" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="11"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="22"/>
-    </row>
-    <row r="45" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="13" t="s">
+    <row r="42" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="11"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="22"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
+      <c r="U42" s="22"/>
+    </row>
+    <row r="43" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="64" t="s">
+      <c r="C43" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="73" t="s">
+      <c r="D43" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="E45" s="59"/>
-      <c r="F45" s="60" t="s">
+      <c r="E43" s="59"/>
+      <c r="F43" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="G45" s="61">
+      <c r="G43" s="61">
         <v>233</v>
       </c>
-      <c r="H45" s="27">
+      <c r="H43" s="27">
         <v>8</v>
       </c>
-      <c r="I45" s="28" t="s">
+      <c r="I43" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="J45" s="27" t="s">
+      <c r="J43" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="K45" s="27" t="s">
+      <c r="K43" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L45" s="27" t="s">
+      <c r="L43" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="M45" s="27" t="s">
+      <c r="M43" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="N45" s="27" t="s">
+      <c r="N43" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="O45" s="27" t="s">
+      <c r="O43" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="P45" s="27" t="s">
+      <c r="P43" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="Q45" s="27" t="s">
+      <c r="Q43" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27"/>
-      <c r="T45" s="27"/>
-      <c r="U45" s="27"/>
+      <c r="R43" s="27"/>
+      <c r="S43" s="27"/>
+      <c r="T43" s="27"/>
+      <c r="U43" s="27"/>
+    </row>
+    <row r="44" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="3"/>
+      <c r="C44" s="31"/>
+    </row>
+    <row r="45" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="G45" s="53">
+        <v>232</v>
+      </c>
+      <c r="H45" s="22">
+        <v>8</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="46" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="3"/>
-      <c r="C46" s="31"/>
+      <c r="B46" s="11" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="47" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="11" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C47" s="62" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="D47" s="71" t="s">
         <v>12</v>
       </c>
       <c r="F47" s="52" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G47" s="53">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H47" s="22">
         <v>8</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="Q47" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C49" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="G49" s="53">
-        <v>231</v>
-      </c>
-      <c r="H49" s="22">
+        <v>152</v>
+      </c>
+      <c r="C48" s="62"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="22"/>
+      <c r="S48" s="22"/>
+      <c r="T48" s="22"/>
+      <c r="U48" s="22"/>
+    </row>
+    <row r="49" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="11"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K49" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L49" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M49" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="N49" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="O49" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="P49" s="22"/>
+      <c r="Q49" s="22"/>
+      <c r="R49" s="22"/>
+      <c r="S49" s="22"/>
+      <c r="T49" s="22"/>
+      <c r="U49" s="22"/>
+    </row>
+    <row r="50" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J50" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="K50" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="L50" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="M50" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="N50" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="O50" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+    </row>
+    <row r="52" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" s="51">
+        <v>122</v>
+      </c>
+      <c r="F52" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="G52" s="53">
+        <v>230</v>
+      </c>
+      <c r="H52" s="22">
         <v>8</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J49" s="1" t="s">
+      <c r="I52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J52" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="K52" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="L52" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="M52" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="N52" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O52" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="P52" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="N49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q49" s="1" t="s">
+      <c r="Q52" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C50" s="62"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M50" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="N50" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="22"/>
-      <c r="S50" s="22"/>
-      <c r="T50" s="22"/>
-      <c r="U50" s="22"/>
-    </row>
-    <row r="51" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="11"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="K51" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="L51" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="M51" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="N51" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="O51" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="22"/>
-      <c r="T51" s="22"/>
-      <c r="U51" s="22"/>
-    </row>
-    <row r="52" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J52" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="K52" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="L52" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="M52" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="N52" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="O52" s="22" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="53" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2722,156 +2806,229 @@
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
     </row>
-    <row r="54" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="D54" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="E54" s="51">
-        <v>122</v>
-      </c>
-      <c r="F54" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="G54" s="53">
-        <v>230</v>
-      </c>
-      <c r="H54" s="22">
-        <v>8</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J54" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="K54" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="L54" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="M54" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="N54" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="O54" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="P54" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q54" s="1" t="s">
+    <row r="54" spans="2:21" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="10"/>
+      <c r="C54" s="64"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="60"/>
+      <c r="G54" s="61"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="27"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="27"/>
+      <c r="O54" s="27"/>
+      <c r="P54" s="27"/>
+      <c r="Q54" s="27"/>
+      <c r="R54" s="27"/>
+      <c r="S54" s="27"/>
+      <c r="T54" s="27"/>
+      <c r="U54" s="27"/>
+    </row>
+    <row r="55" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="11"/>
+      <c r="C55" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="71">
+        <v>77</v>
+      </c>
+      <c r="E55" s="57">
+        <v>119</v>
+      </c>
+      <c r="F55" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="G55" s="58">
+        <v>234</v>
+      </c>
+      <c r="H55" s="22"/>
+      <c r="I55" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J55" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="K55" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="L55" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="M55" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N55" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="O55" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="P55" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q55" s="22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J55" s="22"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="22"/>
-      <c r="O55" s="22"/>
-    </row>
-    <row r="56" spans="2:21" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="10"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="60"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="27"/>
-      <c r="T56" s="27"/>
-      <c r="U56" s="27"/>
-    </row>
-    <row r="57" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="11"/>
-      <c r="C57" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="D57" s="71">
-        <v>77</v>
-      </c>
-      <c r="E57" s="57">
-        <v>119</v>
-      </c>
-      <c r="F57" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="G57" s="58">
-        <v>234</v>
-      </c>
-      <c r="H57" s="22"/>
-      <c r="I57" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J57" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="K57" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="L57" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="M57" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="N57" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="O57" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="P57" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q57" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="S57" s="22"/>
-      <c r="T57" s="22"/>
-      <c r="U57" s="22"/>
-    </row>
-    <row r="58" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="11"/>
-      <c r="C58" s="62"/>
-      <c r="D58" s="71"/>
-      <c r="E58" s="57"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="22"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22"/>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
-      <c r="S58" s="22"/>
-      <c r="T58" s="22"/>
-      <c r="U58" s="22"/>
-    </row>
-    <row r="59" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="S55" s="22"/>
+      <c r="T55" s="22"/>
+      <c r="U55" s="22"/>
+    </row>
+    <row r="56" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="11"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="57"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+      <c r="P56" s="22"/>
+      <c r="Q56" s="22"/>
+      <c r="R56" s="22"/>
+      <c r="S56" s="22"/>
+      <c r="T56" s="22"/>
+      <c r="U56" s="22"/>
+    </row>
+    <row r="57" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="88" t="s">
+        <v>170</v>
+      </c>
+      <c r="D58" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="E58" s="85"/>
+      <c r="F58" s="86" t="s">
+        <v>168</v>
+      </c>
+      <c r="G58" s="87"/>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B59" s="83" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="71">
+        <v>254</v>
+      </c>
+      <c r="E59" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="52">
+        <v>253</v>
+      </c>
+      <c r="G59" s="53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B60" s="83"/>
+      <c r="C60" s="82"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="23"/>
+      <c r="L60" s="23"/>
+      <c r="M60" s="23"/>
+      <c r="N60" s="23"/>
+      <c r="O60" s="23"/>
+      <c r="P60" s="23"/>
+      <c r="Q60" s="23"/>
+      <c r="R60" s="23"/>
+      <c r="S60" s="23"/>
+      <c r="T60" s="23"/>
+      <c r="U60" s="23"/>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B61" s="83" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="82" t="s">
+        <v>164</v>
+      </c>
+      <c r="D61" s="71">
+        <v>239</v>
+      </c>
+      <c r="E61" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="52">
+        <v>237</v>
+      </c>
+      <c r="G61" s="53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B62" s="83"/>
+      <c r="C62" s="82"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="M62" s="23"/>
+      <c r="N62" s="23"/>
+      <c r="O62" s="23"/>
+      <c r="P62" s="23"/>
+      <c r="Q62" s="23"/>
+      <c r="R62" s="23"/>
+      <c r="S62" s="23"/>
+      <c r="T62" s="23"/>
+      <c r="U62" s="23"/>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B63" s="83" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="F63" s="52">
+        <v>211</v>
+      </c>
+      <c r="G63" s="53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B64" s="83"/>
+      <c r="C64" s="82"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="23"/>
+      <c r="L64" s="23"/>
+      <c r="M64" s="23"/>
+      <c r="N64" s="23"/>
+      <c r="O64" s="23"/>
+      <c r="P64" s="23"/>
+      <c r="Q64" s="23"/>
+      <c r="R64" s="23"/>
+      <c r="S64" s="23"/>
+      <c r="T64" s="23"/>
+      <c r="U64" s="23"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65" s="83" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="82" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="I23:J23"/>
@@ -2885,7 +3042,7 @@
     <mergeCell ref="I9:J9"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="62" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="54" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3071,15 +3228,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
section Width Sent with section config
</commit_message>
<xml_diff>
--- a/Support/PGN 5.6.xlsx
+++ b/Support/PGN 5.6.xlsx
@@ -10,7 +10,7 @@
     <sheet name="PGN" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">PGN!$A$1:$Q$73</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PGN!$A$1:$Q$75</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="180">
   <si>
     <t>Src</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>IP_Three</t>
+  </si>
+  <si>
+    <t>SectionDimensions</t>
+  </si>
+  <si>
+    <t>EB</t>
   </si>
 </sst>
 </file>
@@ -913,7 +919,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1147,22 +1153,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1189,6 +1180,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1498,7 +1513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1509,18 +1524,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AG72"/>
+  <dimension ref="B1:AG74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="62" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="62" customWidth="1"/>
     <col min="4" max="4" width="6" style="71" customWidth="1"/>
     <col min="5" max="5" width="5.140625" style="51" customWidth="1"/>
     <col min="6" max="6" width="5.140625" style="52" customWidth="1"/>
@@ -1639,17 +1654,17 @@
       <c r="H3" s="22">
         <v>8</v>
       </c>
-      <c r="I3" s="85" t="s">
+      <c r="I3" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="86"/>
+      <c r="J3" s="98"/>
       <c r="K3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="87" t="s">
+      <c r="L3" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="88"/>
+      <c r="M3" s="100"/>
       <c r="N3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1703,10 +1718,10 @@
       <c r="M5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="89" t="s">
+      <c r="N5" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="89"/>
+      <c r="O5" s="101"/>
       <c r="P5" s="1" t="s">
         <v>35</v>
       </c>
@@ -1795,18 +1810,18 @@
       <c r="H9" s="22">
         <v>8</v>
       </c>
-      <c r="I9" s="90" t="s">
+      <c r="I9" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="84"/>
-      <c r="K9" s="89" t="s">
+      <c r="J9" s="96"/>
+      <c r="K9" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="89"/>
-      <c r="M9" s="89" t="s">
+      <c r="L9" s="101"/>
+      <c r="M9" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="89"/>
+      <c r="N9" s="101"/>
       <c r="O9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2118,164 +2133,205 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="11"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="85"/>
+      <c r="O19" s="85"/>
+      <c r="P19" s="85"/>
+      <c r="Q19" s="85"/>
+      <c r="R19" s="85"/>
+      <c r="S19" s="85"/>
+      <c r="T19" s="85"/>
+      <c r="U19" s="85"/>
+    </row>
     <row r="20" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="11"/>
       <c r="C20" s="62" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="51">
+        <v>127</v>
+      </c>
+      <c r="F20" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="53">
+        <v>235</v>
+      </c>
+      <c r="H20" s="84">
+        <v>16</v>
+      </c>
+      <c r="I20" s="83">
+        <v>1</v>
+      </c>
+      <c r="J20" s="85">
+        <v>2</v>
+      </c>
+      <c r="K20" s="85">
+        <v>3</v>
+      </c>
+      <c r="L20" s="85">
+        <v>4</v>
+      </c>
+      <c r="M20" s="85">
+        <v>5</v>
+      </c>
+      <c r="N20" s="85">
+        <v>6</v>
+      </c>
+      <c r="O20" s="85">
+        <v>7</v>
+      </c>
+      <c r="P20" s="85">
+        <v>8</v>
+      </c>
+      <c r="Q20" s="85">
+        <v>9</v>
+      </c>
+      <c r="R20" s="85">
+        <v>10</v>
+      </c>
+      <c r="S20" s="85">
+        <v>11</v>
+      </c>
+      <c r="T20" s="85">
+        <v>12</v>
+      </c>
+      <c r="U20" s="85">
+        <v>13</v>
+      </c>
+      <c r="V20" s="3">
+        <v>14</v>
+      </c>
+      <c r="W20" s="3">
+        <v>15</v>
+      </c>
+      <c r="X20" s="3">
+        <v>16</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D22" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E22" s="51">
         <v>123</v>
       </c>
-      <c r="F20" s="52" t="s">
+      <c r="F22" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G22" s="53">
         <v>237</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H22" s="22">
         <v>8</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I22" s="2">
         <v>1</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J22" s="1">
         <v>2</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K22" s="1">
         <v>3</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L22" s="1">
         <v>4</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+    <row r="24" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-    </row>
-    <row r="23" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="11"/>
-      <c r="C23" s="62" t="s">
+      <c r="C24" s="64"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+    </row>
+    <row r="25" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="11"/>
+      <c r="C25" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="71">
+      <c r="D25" s="71">
         <v>79</v>
       </c>
-      <c r="E23" s="57">
+      <c r="E25" s="57">
         <v>121</v>
       </c>
-      <c r="F23" s="52" t="s">
+      <c r="F25" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="G23" s="58">
-        <f>HEX2DEC(F23)</f>
+      <c r="G25" s="58">
+        <f>HEX2DEC(F25)</f>
         <v>211</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H25" s="22">
         <v>8</v>
       </c>
-      <c r="I23" s="83" t="s">
+      <c r="I25" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84" t="s">
+      <c r="J25" s="96"/>
+      <c r="K25" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="L23" s="84"/>
-      <c r="M23" s="84" t="s">
+      <c r="L25" s="96"/>
+      <c r="M25" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="N23" s="84"/>
-      <c r="O23" s="22">
+      <c r="N25" s="96"/>
+      <c r="O25" s="22">
         <v>0</v>
       </c>
-      <c r="P23" s="22">
+      <c r="P25" s="22">
         <v>0</v>
       </c>
-      <c r="Q23" s="22" t="s">
+      <c r="Q25" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
-      <c r="U23" s="22"/>
-    </row>
-    <row r="24" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
-    </row>
-    <row r="25" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
+      <c r="R25" s="22"/>
       <c r="S25" s="22"/>
       <c r="T25" s="22"/>
       <c r="U25" s="22"/>
     </row>
     <row r="26" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="11" t="s">
-        <v>155</v>
+      <c r="B26" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="C26" s="62"/>
       <c r="D26" s="71"/>
@@ -2299,7 +2355,7 @@
     </row>
     <row r="27" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C27" s="62"/>
       <c r="D27" s="71"/>
@@ -2322,7 +2378,9 @@
       <c r="U27" s="22"/>
     </row>
     <row r="28" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="11"/>
+      <c r="B28" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="C28" s="62"/>
       <c r="D28" s="71"/>
       <c r="E28" s="51"/>
@@ -2343,113 +2401,115 @@
       <c r="T28" s="22"/>
       <c r="U28" s="22"/>
     </row>
-    <row r="29" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+    <row r="29" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="62"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+    </row>
+    <row r="30" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="11"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
+      <c r="U30" s="22"/>
+    </row>
+    <row r="31" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="61"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-    </row>
-    <row r="30" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="62" t="s">
+      <c r="C31" s="30"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="61"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="27"/>
+      <c r="S31" s="27"/>
+      <c r="T31" s="27"/>
+      <c r="U31" s="27"/>
+    </row>
+    <row r="32" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="71" t="s">
+      <c r="D32" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="57">
+      <c r="E32" s="57">
         <v>124</v>
       </c>
-      <c r="F30" s="52" t="s">
+      <c r="F32" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="58">
+      <c r="G32" s="58">
         <v>214</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="8" t="s">
+    <row r="33" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="11" t="s">
+    <row r="34" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="11" t="s">
+    <row r="35" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="52"/>
-      <c r="G33" s="58"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="22"/>
-      <c r="S33" s="22"/>
-      <c r="T33" s="22"/>
-      <c r="U33" s="22"/>
-    </row>
-    <row r="34" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="58"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="22"/>
-      <c r="U34" s="22"/>
-    </row>
-    <row r="35" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="62"/>
+      <c r="C35" s="31"/>
       <c r="D35" s="71"/>
       <c r="E35" s="57"/>
       <c r="F35" s="52"/>
       <c r="G35" s="58"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="2"/>
+      <c r="I35" s="31"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
       <c r="L35" s="22"/>
@@ -2463,391 +2523,380 @@
       <c r="T35" s="22"/>
       <c r="U35" s="22"/>
     </row>
-    <row r="36" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
+    <row r="36" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="31"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="58"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
+      <c r="U36" s="22"/>
+    </row>
+    <row r="37" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="62"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="22"/>
+      <c r="P37" s="22"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="22"/>
+      <c r="S37" s="22"/>
+      <c r="T37" s="22"/>
+      <c r="U37" s="22"/>
+    </row>
+    <row r="38" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="61"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="27"/>
-      <c r="R36" s="27"/>
-      <c r="S36" s="27"/>
-      <c r="T36" s="27"/>
-      <c r="U36" s="27"/>
-    </row>
-    <row r="37" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="62" t="s">
+      <c r="C38" s="30"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="61"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="27"/>
+      <c r="S38" s="27"/>
+      <c r="T38" s="27"/>
+      <c r="U38" s="27"/>
+    </row>
+    <row r="39" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="D37" s="71" t="s">
+      <c r="D39" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="E37" s="57">
+      <c r="E39" s="57">
         <v>125</v>
       </c>
-      <c r="F37" s="52" t="s">
+      <c r="F39" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="58">
+      <c r="G39" s="58">
         <v>215</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="8" t="s">
+    <row r="40" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="8" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="11" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="41" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="11"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="22"/>
-      <c r="Q42" s="22"/>
-      <c r="R42" s="22"/>
-      <c r="S42" s="22"/>
-      <c r="T42" s="22"/>
-      <c r="U42" s="22"/>
-    </row>
-    <row r="43" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="13" t="s">
+    <row r="44" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="11"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="22"/>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="22"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="22"/>
+      <c r="U44" s="22"/>
+    </row>
+    <row r="45" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C43" s="64" t="s">
+      <c r="C45" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="73" t="s">
+      <c r="D45" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="59"/>
-      <c r="F43" s="60" t="s">
+      <c r="E45" s="59"/>
+      <c r="F45" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="G43" s="61">
+      <c r="G45" s="61">
         <v>233</v>
       </c>
-      <c r="H43" s="27">
+      <c r="H45" s="27">
         <v>8</v>
       </c>
-      <c r="I43" s="28" t="s">
+      <c r="I45" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="J43" s="27" t="s">
+      <c r="J45" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="K43" s="27" t="s">
+      <c r="K45" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L43" s="27" t="s">
+      <c r="L45" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="M43" s="27" t="s">
+      <c r="M45" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="N43" s="27" t="s">
+      <c r="N45" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="O43" s="27" t="s">
+      <c r="O45" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="P43" s="27" t="s">
+      <c r="P45" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="Q43" s="27" t="s">
+      <c r="Q45" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="R43" s="27"/>
-      <c r="S43" s="27"/>
-      <c r="T43" s="27"/>
-      <c r="U43" s="27"/>
-    </row>
-    <row r="44" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="3"/>
-      <c r="C44" s="31"/>
-    </row>
-    <row r="45" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C45" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="G45" s="53">
-        <v>232</v>
-      </c>
-      <c r="H45" s="22">
-        <v>8</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="R45" s="27"/>
+      <c r="S45" s="27"/>
+      <c r="T45" s="27"/>
+      <c r="U45" s="27"/>
     </row>
     <row r="46" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="11" t="s">
-        <v>162</v>
-      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="31"/>
     </row>
     <row r="47" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C47" s="62" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="D47" s="71" t="s">
         <v>12</v>
       </c>
       <c r="F47" s="52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G47" s="53">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H47" s="22">
         <v>8</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="Q47" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="G49" s="53">
+        <v>231</v>
+      </c>
+      <c r="H49" s="22">
+        <v>8</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="62"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="2" t="s">
+      <c r="C50" s="62"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="M50" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="N50" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="O50" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="22"/>
-      <c r="S48" s="22"/>
-      <c r="T48" s="22"/>
-      <c r="U48" s="22"/>
-    </row>
-    <row r="49" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="11"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="22" t="s">
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="22"/>
+      <c r="S50" s="22"/>
+      <c r="T50" s="22"/>
+      <c r="U50" s="22"/>
+    </row>
+    <row r="51" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="11"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="K49" s="22" t="s">
+      <c r="K51" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="L49" s="22" t="s">
+      <c r="L51" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="M49" s="22" t="s">
+      <c r="M51" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="N49" s="22" t="s">
+      <c r="N51" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="O49" s="22" t="s">
+      <c r="O51" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="P49" s="22"/>
-      <c r="Q49" s="22"/>
-      <c r="R49" s="22"/>
-      <c r="S49" s="22"/>
-      <c r="T49" s="22"/>
-      <c r="U49" s="22"/>
-    </row>
-    <row r="50" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J50" s="22" t="s">
+      <c r="P51" s="22"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="22"/>
+      <c r="S51" s="22"/>
+      <c r="T51" s="22"/>
+      <c r="U51" s="22"/>
+    </row>
+    <row r="52" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J52" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="K50" s="22" t="s">
+      <c r="K52" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="L50" s="22" t="s">
+      <c r="L52" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="M50" s="22" t="s">
+      <c r="M52" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="N50" s="22" t="s">
+      <c r="N52" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="O50" s="22" t="s">
+      <c r="O52" s="22" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-    </row>
-    <row r="52" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C52" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" s="51">
-        <v>122</v>
-      </c>
-      <c r="F52" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="G52" s="53">
-        <v>230</v>
-      </c>
-      <c r="H52" s="22">
-        <v>8</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J52" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="K52" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="L52" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="M52" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="N52" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="O52" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="53" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2858,120 +2907,131 @@
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
     </row>
-    <row r="54" spans="2:21" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="10"/>
-      <c r="C54" s="64"/>
-      <c r="D54" s="73"/>
-      <c r="E54" s="59"/>
-      <c r="F54" s="60"/>
-      <c r="G54" s="61"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="27"/>
-      <c r="M54" s="27"/>
-      <c r="N54" s="27"/>
-      <c r="O54" s="27"/>
-      <c r="P54" s="27"/>
-      <c r="Q54" s="27"/>
-      <c r="R54" s="27"/>
-      <c r="S54" s="27"/>
-      <c r="T54" s="27"/>
-      <c r="U54" s="27"/>
-    </row>
-    <row r="55" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="11"/>
-      <c r="C55" s="62" t="s">
+    <row r="54" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" s="51">
+        <v>122</v>
+      </c>
+      <c r="F54" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="G54" s="53">
+        <v>230</v>
+      </c>
+      <c r="H54" s="22">
+        <v>8</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J54" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="K54" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="L54" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="M54" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="N54" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O54" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="22"/>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
+    </row>
+    <row r="56" spans="2:21" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="10"/>
+      <c r="C56" s="64"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="59"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="61"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="27"/>
+      <c r="O56" s="27"/>
+      <c r="P56" s="27"/>
+      <c r="Q56" s="27"/>
+      <c r="R56" s="27"/>
+      <c r="S56" s="27"/>
+      <c r="T56" s="27"/>
+      <c r="U56" s="27"/>
+    </row>
+    <row r="57" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="11"/>
+      <c r="C57" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="71">
+      <c r="D57" s="71">
         <v>77</v>
       </c>
-      <c r="E55" s="57">
+      <c r="E57" s="57">
         <v>119</v>
       </c>
-      <c r="F55" s="52" t="s">
+      <c r="F57" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="G55" s="58">
+      <c r="G57" s="58">
         <v>234</v>
       </c>
-      <c r="H55" s="22"/>
-      <c r="I55" s="2" t="s">
+      <c r="H57" s="22"/>
+      <c r="I57" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J55" s="22" t="s">
+      <c r="J57" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="K55" s="22" t="s">
+      <c r="K57" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="L55" s="22" t="s">
+      <c r="L57" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="M55" s="22" t="s">
+      <c r="M57" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="N55" s="22" t="s">
+      <c r="N57" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="O55" s="22" t="s">
+      <c r="O57" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="P55" s="22" t="s">
+      <c r="P57" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="Q55" s="22" t="s">
+      <c r="Q57" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="S55" s="22"/>
-      <c r="T55" s="22"/>
-      <c r="U55" s="22"/>
-    </row>
-    <row r="56" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="11"/>
-      <c r="C56" s="62"/>
-      <c r="D56" s="71"/>
-      <c r="E56" s="57"/>
-      <c r="F56" s="52"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="22"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="22"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="22"/>
-      <c r="O56" s="22"/>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="22"/>
-      <c r="R56" s="22"/>
-      <c r="S56" s="22"/>
-      <c r="T56" s="22"/>
-      <c r="U56" s="22"/>
-    </row>
-    <row r="57" spans="2:21" s="91" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="92"/>
-      <c r="C57" s="93"/>
-      <c r="D57" s="94"/>
-      <c r="E57" s="95"/>
-      <c r="F57" s="96"/>
-      <c r="G57" s="81"/>
-      <c r="H57" s="97"/>
-      <c r="I57" s="98"/>
-      <c r="J57" s="97"/>
-      <c r="K57" s="97"/>
-      <c r="L57" s="97"/>
-      <c r="M57" s="97"/>
-      <c r="N57" s="97"/>
-      <c r="O57" s="97"/>
-      <c r="P57" s="97"/>
-      <c r="Q57" s="97"/>
-      <c r="R57" s="97"/>
-      <c r="S57" s="97"/>
-      <c r="T57" s="97"/>
-      <c r="U57" s="97"/>
+      <c r="S57" s="22"/>
+      <c r="T57" s="22"/>
+      <c r="U57" s="22"/>
     </row>
     <row r="58" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="11"/>
@@ -2980,60 +3040,42 @@
       <c r="E58" s="57"/>
       <c r="F58" s="52"/>
       <c r="G58" s="58"/>
-      <c r="H58" s="74"/>
-      <c r="I58" s="75"/>
-      <c r="J58" s="74"/>
-      <c r="K58" s="74"/>
-      <c r="L58" s="74"/>
-      <c r="M58" s="74"/>
-      <c r="N58" s="74"/>
-      <c r="O58" s="74"/>
-      <c r="P58" s="74"/>
-      <c r="Q58" s="74"/>
-      <c r="R58" s="74"/>
-      <c r="S58" s="74"/>
-      <c r="T58" s="74"/>
-      <c r="U58" s="74"/>
-    </row>
-    <row r="59" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="99" t="s">
-        <v>171</v>
-      </c>
-      <c r="C59" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="D59" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="57"/>
-      <c r="F59" s="52"/>
-      <c r="G59" s="58">
-        <v>200</v>
-      </c>
-      <c r="H59" s="74">
-        <v>3</v>
-      </c>
-      <c r="I59" s="75" t="s">
-        <v>173</v>
-      </c>
-      <c r="J59" s="74">
-        <v>0</v>
-      </c>
-      <c r="K59" s="74">
-        <v>0</v>
-      </c>
-      <c r="L59" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="M59" s="74"/>
-      <c r="N59" s="74"/>
-      <c r="O59" s="74"/>
-      <c r="P59" s="74"/>
-      <c r="Q59" s="74"/>
-      <c r="R59" s="74"/>
-      <c r="S59" s="74"/>
-      <c r="T59" s="74"/>
-      <c r="U59" s="74"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="22"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="22"/>
+      <c r="S58" s="22"/>
+      <c r="T58" s="22"/>
+      <c r="U58" s="22"/>
+    </row>
+    <row r="59" spans="2:21" s="86" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="87"/>
+      <c r="C59" s="88"/>
+      <c r="D59" s="89"/>
+      <c r="E59" s="90"/>
+      <c r="F59" s="91"/>
+      <c r="G59" s="81"/>
+      <c r="H59" s="92"/>
+      <c r="I59" s="93"/>
+      <c r="J59" s="92"/>
+      <c r="K59" s="92"/>
+      <c r="L59" s="92"/>
+      <c r="M59" s="92"/>
+      <c r="N59" s="92"/>
+      <c r="O59" s="92"/>
+      <c r="P59" s="92"/>
+      <c r="Q59" s="92"/>
+      <c r="R59" s="92"/>
+      <c r="S59" s="92"/>
+      <c r="T59" s="92"/>
+      <c r="U59" s="92"/>
     </row>
     <row r="60" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="11"/>
@@ -3057,10 +3099,12 @@
       <c r="T60" s="74"/>
       <c r="U60" s="74"/>
     </row>
-    <row r="61" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="11"/>
+    <row r="61" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="94" t="s">
+        <v>171</v>
+      </c>
       <c r="C61" s="62" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D61" s="71" t="s">
         <v>12</v>
@@ -3068,29 +3112,25 @@
       <c r="E61" s="57"/>
       <c r="F61" s="52"/>
       <c r="G61" s="58">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H61" s="74">
-        <v>5</v>
-      </c>
-      <c r="I61" s="75">
-        <v>201</v>
+        <v>3</v>
+      </c>
+      <c r="I61" s="75" t="s">
+        <v>173</v>
       </c>
       <c r="J61" s="74">
-        <v>201</v>
-      </c>
-      <c r="K61" s="74" t="s">
-        <v>175</v>
+        <v>0</v>
+      </c>
+      <c r="K61" s="74">
+        <v>0</v>
       </c>
       <c r="L61" s="74" t="s">
-        <v>176</v>
-      </c>
-      <c r="M61" s="74" t="s">
-        <v>177</v>
-      </c>
-      <c r="N61" s="74" t="s">
         <v>20</v>
       </c>
+      <c r="M61" s="74"/>
+      <c r="N61" s="74"/>
       <c r="O61" s="74"/>
       <c r="P61" s="74"/>
       <c r="Q61" s="74"/>
@@ -3123,18 +3163,38 @@
     </row>
     <row r="63" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="11"/>
-      <c r="C63" s="62"/>
-      <c r="D63" s="71"/>
+      <c r="C63" s="62" t="s">
+        <v>174</v>
+      </c>
+      <c r="D63" s="71" t="s">
+        <v>12</v>
+      </c>
       <c r="E63" s="57"/>
       <c r="F63" s="52"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="74"/>
-      <c r="I63" s="75"/>
-      <c r="J63" s="74"/>
-      <c r="K63" s="74"/>
-      <c r="L63" s="74"/>
-      <c r="M63" s="74"/>
-      <c r="N63" s="74"/>
+      <c r="G63" s="58">
+        <v>201</v>
+      </c>
+      <c r="H63" s="74">
+        <v>5</v>
+      </c>
+      <c r="I63" s="75">
+        <v>201</v>
+      </c>
+      <c r="J63" s="74">
+        <v>201</v>
+      </c>
+      <c r="K63" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="L63" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="M63" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="N63" s="74" t="s">
+        <v>20</v>
+      </c>
       <c r="O63" s="74"/>
       <c r="P63" s="74"/>
       <c r="Q63" s="74"/>
@@ -3143,76 +3203,82 @@
       <c r="T63" s="74"/>
       <c r="U63" s="74"/>
     </row>
-    <row r="64" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="82" t="s">
+    <row r="64" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="11"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="57"/>
+      <c r="F64" s="52"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="74"/>
+      <c r="I64" s="75"/>
+      <c r="J64" s="74"/>
+      <c r="K64" s="74"/>
+      <c r="L64" s="74"/>
+      <c r="M64" s="74"/>
+      <c r="N64" s="74"/>
+      <c r="O64" s="74"/>
+      <c r="P64" s="74"/>
+      <c r="Q64" s="74"/>
+      <c r="R64" s="74"/>
+      <c r="S64" s="74"/>
+      <c r="T64" s="74"/>
+      <c r="U64" s="74"/>
+    </row>
+    <row r="65" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="11"/>
+      <c r="C65" s="62"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="57"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="74"/>
+      <c r="I65" s="75"/>
+      <c r="J65" s="74"/>
+      <c r="K65" s="74"/>
+      <c r="L65" s="74"/>
+      <c r="M65" s="74"/>
+      <c r="N65" s="74"/>
+      <c r="O65" s="74"/>
+      <c r="P65" s="74"/>
+      <c r="Q65" s="74"/>
+      <c r="R65" s="74"/>
+      <c r="S65" s="74"/>
+      <c r="T65" s="74"/>
+      <c r="U65" s="74"/>
+    </row>
+    <row r="66" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="D65" s="78" t="s">
+      <c r="D67" s="78" t="s">
         <v>169</v>
       </c>
-      <c r="E65" s="79"/>
-      <c r="F65" s="80" t="s">
+      <c r="E67" s="79"/>
+      <c r="F67" s="80" t="s">
         <v>168</v>
       </c>
-      <c r="G65" s="81"/>
-    </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B66" s="77" t="s">
-        <v>136</v>
-      </c>
-      <c r="C66" s="76" t="s">
-        <v>165</v>
-      </c>
-      <c r="D66" s="71">
-        <v>254</v>
-      </c>
-      <c r="E66" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="F66" s="52">
-        <v>253</v>
-      </c>
-      <c r="G66" s="53" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B67" s="77"/>
-      <c r="C67" s="76"/>
-      <c r="H67" s="24"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
-      <c r="M67" s="23"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="23"/>
-      <c r="P67" s="23"/>
-      <c r="Q67" s="23"/>
-      <c r="R67" s="23"/>
-      <c r="S67" s="23"/>
-      <c r="T67" s="23"/>
-      <c r="U67" s="23"/>
+      <c r="G67" s="81"/>
     </row>
     <row r="68" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B68" s="77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C68" s="76" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D68" s="71">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="E68" s="51" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="F68" s="52">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="G68" s="53" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="2:21" x14ac:dyDescent="0.2">
@@ -3235,16 +3301,22 @@
     </row>
     <row r="70" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B70" s="77" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="C70" s="76" t="s">
-        <v>166</v>
+        <v>164</v>
+      </c>
+      <c r="D70" s="71">
+        <v>239</v>
+      </c>
+      <c r="E70" s="51" t="s">
+        <v>41</v>
       </c>
       <c r="F70" s="52">
-        <v>211</v>
+        <v>237</v>
       </c>
       <c r="G70" s="53" t="s">
-        <v>131</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="2:21" x14ac:dyDescent="0.2">
@@ -3267,17 +3339,49 @@
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B72" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="F72" s="52">
+        <v>211</v>
+      </c>
+      <c r="G72" s="53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B73" s="77"/>
+      <c r="C73" s="76"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="23"/>
+      <c r="N73" s="23"/>
+      <c r="O73" s="23"/>
+      <c r="P73" s="23"/>
+      <c r="Q73" s="23"/>
+      <c r="R73" s="23"/>
+      <c r="S73" s="23"/>
+      <c r="T73" s="23"/>
+      <c r="U73" s="23"/>
+    </row>
+    <row r="74" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B74" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="C72" s="76" t="s">
+      <c r="C74" s="76" t="s">
         <v>167</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N5:O5"/>
@@ -3291,12 +3395,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3464,15 +3565,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3496,17 +3608,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
pgn, brightness reset, start speed
</commit_message>
<xml_diff>
--- a/Support/PGN 5.6.xlsx
+++ b/Support/PGN 5.6.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="182">
   <si>
     <t>Src</t>
   </si>
@@ -568,6 +568,12 @@
   </si>
   <si>
     <t>EB</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>crc</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1528,7 +1534,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomLeft" activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2168,7 +2174,7 @@
         <v>235</v>
       </c>
       <c r="H20" s="84">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I20" s="83">
         <v>1</v>
@@ -2219,7 +2225,10 @@
         <v>16</v>
       </c>
       <c r="Y20" s="3" t="s">
-        <v>20</v>
+        <v>180</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3395,9 +3404,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3565,26 +3577,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3608,9 +3609,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
16 bit config pgn for section widths
</commit_message>
<xml_diff>
--- a/Support/PGN 5.6.xlsx
+++ b/Support/PGN 5.6.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="197">
   <si>
     <t>Src</t>
   </si>
@@ -570,10 +570,55 @@
     <t>EB</t>
   </si>
   <si>
-    <t>num</t>
-  </si>
-  <si>
-    <t>crc</t>
+    <t>1Hi</t>
+  </si>
+  <si>
+    <t>2Hi</t>
+  </si>
+  <si>
+    <t>3Hi</t>
+  </si>
+  <si>
+    <t>4Hi</t>
+  </si>
+  <si>
+    <t>5Hi</t>
+  </si>
+  <si>
+    <t>6Hi</t>
+  </si>
+  <si>
+    <t>7Hi</t>
+  </si>
+  <si>
+    <t>8Hi</t>
+  </si>
+  <si>
+    <t>9Hi</t>
+  </si>
+  <si>
+    <t>10Hi</t>
+  </si>
+  <si>
+    <t>11Hi</t>
+  </si>
+  <si>
+    <t>12Hi</t>
+  </si>
+  <si>
+    <t>13Hi</t>
+  </si>
+  <si>
+    <t>14Hi</t>
+  </si>
+  <si>
+    <t>15Hi</t>
+  </si>
+  <si>
+    <t>16Hi</t>
+  </si>
+  <si>
+    <t>NumSec</t>
   </si>
 </sst>
 </file>
@@ -925,7 +970,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -973,8 +1018,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
@@ -1052,8 +1095,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1187,6 +1228,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1209,6 +1256,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1519,7 +1584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1530,46 +1595,45 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AG74"/>
+  <dimension ref="B1:AP74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z21" sqref="Z21"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="62" customWidth="1"/>
-    <col min="4" max="4" width="6" style="71" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" style="51" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="52" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="53" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="6" style="67" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" style="47" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="48" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="49" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="20" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" style="2" customWidth="1"/>
     <col min="10" max="16" width="14.42578125" style="1" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="21" width="5.5703125" style="1" customWidth="1"/>
-    <col min="22" max="33" width="5.5703125" style="3" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="3"/>
+    <col min="18" max="40" width="5.7109375" style="92" customWidth="1"/>
+    <col min="41" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" s="14" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:40" s="14" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
       <c r="B1" s="7"/>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="61" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="30" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="16" t="s">
@@ -1602,111 +1666,143 @@
       <c r="Q1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-    </row>
-    <row r="2" spans="2:24" s="39" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="38"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-    </row>
-    <row r="3" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S1" s="102"/>
+      <c r="T1" s="102"/>
+      <c r="U1" s="102"/>
+      <c r="V1" s="102"/>
+      <c r="W1" s="102"/>
+      <c r="X1" s="102"/>
+      <c r="Y1" s="103"/>
+      <c r="Z1" s="103"/>
+      <c r="AA1" s="103"/>
+      <c r="AB1" s="103"/>
+      <c r="AC1" s="103"/>
+      <c r="AD1" s="103"/>
+      <c r="AE1" s="103"/>
+      <c r="AF1" s="103"/>
+      <c r="AG1" s="103"/>
+      <c r="AH1" s="103"/>
+      <c r="AI1" s="103"/>
+      <c r="AJ1" s="103"/>
+      <c r="AK1" s="103"/>
+      <c r="AL1" s="103"/>
+      <c r="AM1" s="103"/>
+      <c r="AN1" s="103"/>
+    </row>
+    <row r="2" spans="2:40" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="36"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
+      <c r="X2" s="91"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="105"/>
+      <c r="AE2" s="105"/>
+      <c r="AF2" s="105"/>
+      <c r="AG2" s="105"/>
+      <c r="AH2" s="105"/>
+      <c r="AI2" s="105"/>
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="105"/>
+      <c r="AM2" s="105"/>
+      <c r="AN2" s="105"/>
+    </row>
+    <row r="3" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="33">
         <v>127</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="33">
+      <c r="G3" s="31">
         <f>HEX2DEC(F3)</f>
         <v>254</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="20">
         <v>8</v>
       </c>
-      <c r="I3" s="97" t="s">
+      <c r="I3" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="98"/>
-      <c r="K3" s="21" t="s">
+      <c r="J3" s="96"/>
+      <c r="K3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="99" t="s">
+      <c r="L3" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="100"/>
+      <c r="M3" s="98"/>
       <c r="N3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-    </row>
-    <row r="5" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R3" s="106"/>
+      <c r="S3" s="106"/>
+    </row>
+    <row r="5" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="47">
         <v>127</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="49">
         <f>HEX2DEC(F5)</f>
         <v>252</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="20">
         <v>8</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1724,10 +1820,10 @@
       <c r="M5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="101" t="s">
+      <c r="N5" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="101"/>
+      <c r="O5" s="99"/>
       <c r="P5" s="1" t="s">
         <v>35</v>
       </c>
@@ -1735,32 +1831,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="47">
         <v>127</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="49">
         <f>HEX2DEC(F7)</f>
         <v>251</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="20">
         <v>8</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1791,43 +1887,43 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="62" t="s">
+    <row r="9" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="47">
         <v>126</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="49">
         <f>HEX2DEC(F9)</f>
         <v>253</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="20">
         <v>8</v>
       </c>
-      <c r="I9" s="102" t="s">
+      <c r="I9" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="96"/>
-      <c r="K9" s="101" t="s">
+      <c r="J9" s="94"/>
+      <c r="K9" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101" t="s">
+      <c r="L9" s="99"/>
+      <c r="M9" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="101"/>
+      <c r="N9" s="99"/>
       <c r="O9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1838,23 +1934,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="62" t="s">
+    <row r="11" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="47">
         <v>126</v>
       </c>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G11" s="49">
         <v>250</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="20">
         <v>8</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -1885,70 +1981,108 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:24" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:40" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-    </row>
-    <row r="13" spans="2:24" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="59"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="23"/>
+      <c r="AC12" s="23"/>
+      <c r="AD12" s="23"/>
+      <c r="AE12" s="23"/>
+      <c r="AF12" s="23"/>
+      <c r="AG12" s="23"/>
+      <c r="AH12" s="23"/>
+      <c r="AI12" s="23"/>
+      <c r="AJ12" s="23"/>
+      <c r="AK12" s="23"/>
+      <c r="AL12" s="23"/>
+      <c r="AM12" s="23"/>
+      <c r="AN12" s="23"/>
+    </row>
+    <row r="13" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="22"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
-      <c r="U13" s="22"/>
-    </row>
-    <row r="14" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="62" t="s">
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="91"/>
+      <c r="S13" s="91"/>
+      <c r="T13" s="91"/>
+      <c r="U13" s="91"/>
+      <c r="V13" s="91"/>
+      <c r="W13" s="91"/>
+      <c r="X13" s="91"/>
+      <c r="Y13" s="91"/>
+      <c r="Z13" s="91"/>
+      <c r="AA13" s="91"/>
+      <c r="AB13" s="91"/>
+      <c r="AC13" s="91"/>
+      <c r="AD13" s="91"/>
+      <c r="AE13" s="91"/>
+      <c r="AF13" s="91"/>
+      <c r="AG13" s="91"/>
+      <c r="AH13" s="91"/>
+      <c r="AI13" s="91"/>
+      <c r="AJ13" s="91"/>
+      <c r="AK13" s="91"/>
+      <c r="AL13" s="91"/>
+      <c r="AM13" s="91"/>
+      <c r="AN13" s="91"/>
+    </row>
+    <row r="14" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="51">
+      <c r="E14" s="47">
         <v>127</v>
       </c>
-      <c r="F14" s="52" t="s">
+      <c r="F14" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="49">
         <f>HEX2DEC(F14)</f>
         <v>239</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="20">
         <v>8</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -1960,7 +2094,7 @@
       <c r="K14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="L14" s="19" t="s">
         <v>44</v>
       </c>
       <c r="M14" s="1" t="s">
@@ -1969,42 +2103,42 @@
       <c r="N14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="O14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:40" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="2:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="71" t="s">
+      <c r="D16" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="51">
+      <c r="E16" s="47">
         <v>127</v>
       </c>
-      <c r="F16" s="52" t="s">
+      <c r="F16" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="53">
+      <c r="G16" s="49">
         <f>HEX2DEC(F16)</f>
         <v>238</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="20">
         <v>8</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -2035,32 +2169,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="51">
+      <c r="E18" s="47">
         <v>127</v>
       </c>
-      <c r="F18" s="52" t="s">
+      <c r="F18" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="49">
         <f t="shared" ref="G18" si="0">HEX2DEC(F18)</f>
         <v>236</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="20">
         <v>24</v>
       </c>
       <c r="I18" s="2">
@@ -2090,165 +2224,209 @@
       <c r="Q18" s="1">
         <v>9</v>
       </c>
-      <c r="R18" s="1">
+      <c r="R18" s="92">
         <v>10</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S18" s="92">
         <v>11</v>
       </c>
-      <c r="T18" s="1">
+      <c r="T18" s="92">
         <v>12</v>
       </c>
-      <c r="U18" s="1">
+      <c r="U18" s="92">
         <v>13</v>
       </c>
-      <c r="V18" s="3">
+      <c r="V18" s="92">
         <v>14</v>
       </c>
-      <c r="W18" s="3">
+      <c r="W18" s="92">
         <v>15</v>
       </c>
-      <c r="X18" s="3">
+      <c r="X18" s="92">
         <v>16</v>
       </c>
-      <c r="Y18" s="3">
+      <c r="Y18" s="92">
         <v>17</v>
       </c>
-      <c r="Z18" s="3">
+      <c r="Z18" s="92">
         <v>18</v>
       </c>
-      <c r="AA18" s="3">
+      <c r="AA18" s="92">
         <v>19</v>
       </c>
-      <c r="AB18" s="3">
+      <c r="AB18" s="92">
         <v>20</v>
       </c>
-      <c r="AC18" s="3">
+      <c r="AC18" s="92">
         <v>21</v>
       </c>
-      <c r="AD18" s="3">
+      <c r="AD18" s="92">
         <v>22</v>
       </c>
-      <c r="AE18" s="3">
+      <c r="AE18" s="92">
         <v>23</v>
       </c>
-      <c r="AF18" s="3">
+      <c r="AF18" s="92">
         <v>24</v>
       </c>
-      <c r="AG18" s="3" t="s">
+      <c r="AG18" s="92" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="11"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85"/>
-      <c r="R19" s="85"/>
-      <c r="S19" s="85"/>
-      <c r="T19" s="85"/>
-      <c r="U19" s="85"/>
-    </row>
-    <row r="20" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="80"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="81"/>
+      <c r="Q19" s="81"/>
+    </row>
+    <row r="20" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="11"/>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E20" s="47">
         <v>127</v>
       </c>
-      <c r="F20" s="52" t="s">
+      <c r="F20" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G20" s="49">
         <v>235</v>
       </c>
-      <c r="H20" s="84">
-        <v>17</v>
-      </c>
-      <c r="I20" s="83">
+      <c r="H20" s="80">
+        <v>33</v>
+      </c>
+      <c r="I20" s="79">
         <v>1</v>
       </c>
-      <c r="J20" s="85">
+      <c r="J20" s="81" t="s">
+        <v>180</v>
+      </c>
+      <c r="K20" s="81">
         <v>2</v>
       </c>
-      <c r="K20" s="85">
+      <c r="L20" s="81" t="s">
+        <v>181</v>
+      </c>
+      <c r="M20" s="81">
         <v>3</v>
       </c>
-      <c r="L20" s="85">
+      <c r="N20" s="81" t="s">
+        <v>182</v>
+      </c>
+      <c r="O20" s="81">
         <v>4</v>
       </c>
-      <c r="M20" s="85">
+      <c r="P20" s="81" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q20" s="81">
         <v>5</v>
       </c>
-      <c r="N20" s="85">
+      <c r="R20" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="S20" s="92">
         <v>6</v>
       </c>
-      <c r="O20" s="85">
+      <c r="T20" s="92" t="s">
+        <v>185</v>
+      </c>
+      <c r="U20" s="92">
         <v>7</v>
       </c>
-      <c r="P20" s="85">
+      <c r="V20" s="92" t="s">
+        <v>186</v>
+      </c>
+      <c r="W20" s="92">
         <v>8</v>
       </c>
-      <c r="Q20" s="85">
+      <c r="X20" s="92" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y20" s="92">
         <v>9</v>
       </c>
-      <c r="R20" s="85">
+      <c r="Z20" s="92" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA20" s="92">
         <v>10</v>
       </c>
-      <c r="S20" s="85">
+      <c r="AB20" s="92" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC20" s="92">
         <v>11</v>
       </c>
-      <c r="T20" s="85">
+      <c r="AD20" s="92" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE20" s="92">
         <v>12</v>
       </c>
-      <c r="U20" s="85">
+      <c r="AF20" s="92" t="s">
+        <v>191</v>
+      </c>
+      <c r="AG20" s="92">
         <v>13</v>
       </c>
-      <c r="V20" s="3">
+      <c r="AH20" s="92" t="s">
+        <v>192</v>
+      </c>
+      <c r="AI20" s="92">
         <v>14</v>
       </c>
-      <c r="W20" s="3">
+      <c r="AJ20" s="92" t="s">
+        <v>193</v>
+      </c>
+      <c r="AK20" s="92">
         <v>15</v>
       </c>
-      <c r="X20" s="3">
+      <c r="AL20" s="92" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM20" s="92">
         <v>16</v>
       </c>
-      <c r="Y20" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="Z20" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="62" t="s">
+      <c r="AN20" s="92" t="s">
+        <v>195</v>
+      </c>
+      <c r="AO20" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="AP20" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="71" t="s">
+      <c r="D22" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="51">
+      <c r="E22" s="47">
         <v>123</v>
       </c>
-      <c r="F22" s="52" t="s">
+      <c r="F22" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="53">
+      <c r="G22" s="49">
         <v>237</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="20">
         <v>8</v>
       </c>
       <c r="I22" s="2">
@@ -2267,473 +2445,739 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:42" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="U24" s="27"/>
-    </row>
-    <row r="25" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="60"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="25"/>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="25"/>
+      <c r="Z24" s="25"/>
+      <c r="AA24" s="25"/>
+      <c r="AB24" s="25"/>
+      <c r="AC24" s="25"/>
+      <c r="AD24" s="25"/>
+      <c r="AE24" s="25"/>
+      <c r="AF24" s="25"/>
+      <c r="AG24" s="25"/>
+      <c r="AH24" s="25"/>
+      <c r="AI24" s="25"/>
+      <c r="AJ24" s="25"/>
+      <c r="AK24" s="25"/>
+      <c r="AL24" s="25"/>
+      <c r="AM24" s="25"/>
+      <c r="AN24" s="25"/>
+    </row>
+    <row r="25" spans="2:42" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="11"/>
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="D25" s="71">
+      <c r="D25" s="67">
         <v>79</v>
       </c>
-      <c r="E25" s="57">
+      <c r="E25" s="53">
         <v>121</v>
       </c>
-      <c r="F25" s="52" t="s">
+      <c r="F25" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="G25" s="58">
+      <c r="G25" s="54">
         <f>HEX2DEC(F25)</f>
         <v>211</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="20">
         <v>8</v>
       </c>
-      <c r="I25" s="95" t="s">
+      <c r="I25" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="J25" s="96"/>
-      <c r="K25" s="96" t="s">
+      <c r="J25" s="94"/>
+      <c r="K25" s="94" t="s">
         <v>133</v>
       </c>
-      <c r="L25" s="96"/>
-      <c r="M25" s="96" t="s">
+      <c r="L25" s="94"/>
+      <c r="M25" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="N25" s="96"/>
-      <c r="O25" s="22">
+      <c r="N25" s="94"/>
+      <c r="O25" s="20">
         <v>0</v>
       </c>
-      <c r="P25" s="22">
+      <c r="P25" s="20">
         <v>0</v>
       </c>
-      <c r="Q25" s="22" t="s">
+      <c r="Q25" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="22"/>
-      <c r="U25" s="22"/>
-    </row>
-    <row r="26" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R25" s="91"/>
+      <c r="S25" s="91"/>
+      <c r="T25" s="91"/>
+      <c r="U25" s="91"/>
+      <c r="V25" s="91"/>
+      <c r="W25" s="91"/>
+      <c r="X25" s="91"/>
+      <c r="Y25" s="91"/>
+      <c r="Z25" s="91"/>
+      <c r="AA25" s="91"/>
+      <c r="AB25" s="91"/>
+      <c r="AC25" s="91"/>
+      <c r="AD25" s="91"/>
+      <c r="AE25" s="91"/>
+      <c r="AF25" s="91"/>
+      <c r="AG25" s="91"/>
+      <c r="AH25" s="91"/>
+      <c r="AI25" s="91"/>
+      <c r="AJ25" s="91"/>
+      <c r="AK25" s="91"/>
+      <c r="AL25" s="91"/>
+      <c r="AM25" s="91"/>
+      <c r="AN25" s="91"/>
+    </row>
+    <row r="26" spans="2:42" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="22"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="22"/>
-      <c r="T26" s="22"/>
-      <c r="U26" s="22"/>
-    </row>
-    <row r="27" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R26" s="92"/>
+      <c r="S26" s="91"/>
+      <c r="T26" s="91"/>
+      <c r="U26" s="91"/>
+      <c r="V26" s="91"/>
+      <c r="W26" s="91"/>
+      <c r="X26" s="91"/>
+      <c r="Y26" s="91"/>
+      <c r="Z26" s="91"/>
+      <c r="AA26" s="91"/>
+      <c r="AB26" s="91"/>
+      <c r="AC26" s="91"/>
+      <c r="AD26" s="91"/>
+      <c r="AE26" s="91"/>
+      <c r="AF26" s="91"/>
+      <c r="AG26" s="91"/>
+      <c r="AH26" s="91"/>
+      <c r="AI26" s="91"/>
+      <c r="AJ26" s="91"/>
+      <c r="AK26" s="91"/>
+      <c r="AL26" s="91"/>
+      <c r="AM26" s="91"/>
+      <c r="AN26" s="91"/>
+    </row>
+    <row r="27" spans="2:42" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="22"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="20"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="22"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="22"/>
-    </row>
-    <row r="28" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R27" s="92"/>
+      <c r="S27" s="91"/>
+      <c r="T27" s="91"/>
+      <c r="U27" s="91"/>
+      <c r="V27" s="91"/>
+      <c r="W27" s="91"/>
+      <c r="X27" s="91"/>
+      <c r="Y27" s="91"/>
+      <c r="Z27" s="91"/>
+      <c r="AA27" s="91"/>
+      <c r="AB27" s="91"/>
+      <c r="AC27" s="91"/>
+      <c r="AD27" s="91"/>
+      <c r="AE27" s="91"/>
+      <c r="AF27" s="91"/>
+      <c r="AG27" s="91"/>
+      <c r="AH27" s="91"/>
+      <c r="AI27" s="91"/>
+      <c r="AJ27" s="91"/>
+      <c r="AK27" s="91"/>
+      <c r="AL27" s="91"/>
+      <c r="AM27" s="91"/>
+      <c r="AN27" s="91"/>
+    </row>
+    <row r="28" spans="2:42" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="22"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="22"/>
-    </row>
-    <row r="29" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R28" s="92"/>
+      <c r="S28" s="91"/>
+      <c r="T28" s="91"/>
+      <c r="U28" s="91"/>
+      <c r="V28" s="91"/>
+      <c r="W28" s="91"/>
+      <c r="X28" s="91"/>
+      <c r="Y28" s="91"/>
+      <c r="Z28" s="91"/>
+      <c r="AA28" s="91"/>
+      <c r="AB28" s="91"/>
+      <c r="AC28" s="91"/>
+      <c r="AD28" s="91"/>
+      <c r="AE28" s="91"/>
+      <c r="AF28" s="91"/>
+      <c r="AG28" s="91"/>
+      <c r="AH28" s="91"/>
+      <c r="AI28" s="91"/>
+      <c r="AJ28" s="91"/>
+      <c r="AK28" s="91"/>
+      <c r="AL28" s="91"/>
+      <c r="AM28" s="91"/>
+      <c r="AN28" s="91"/>
+    </row>
+    <row r="29" spans="2:42" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="22"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="20"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="22"/>
-      <c r="T29" s="22"/>
-      <c r="U29" s="22"/>
-    </row>
-    <row r="30" spans="2:33" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R29" s="92"/>
+      <c r="S29" s="91"/>
+      <c r="T29" s="91"/>
+      <c r="U29" s="91"/>
+      <c r="V29" s="91"/>
+      <c r="W29" s="91"/>
+      <c r="X29" s="91"/>
+      <c r="Y29" s="91"/>
+      <c r="Z29" s="91"/>
+      <c r="AA29" s="91"/>
+      <c r="AB29" s="91"/>
+      <c r="AC29" s="91"/>
+      <c r="AD29" s="91"/>
+      <c r="AE29" s="91"/>
+      <c r="AF29" s="91"/>
+      <c r="AG29" s="91"/>
+      <c r="AH29" s="91"/>
+      <c r="AI29" s="91"/>
+      <c r="AJ29" s="91"/>
+      <c r="AK29" s="91"/>
+      <c r="AL29" s="91"/>
+      <c r="AM29" s="91"/>
+      <c r="AN29" s="91"/>
+    </row>
+    <row r="30" spans="2:42" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="22"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="20"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="22"/>
-      <c r="T30" s="22"/>
-      <c r="U30" s="22"/>
-    </row>
-    <row r="31" spans="2:33" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R30" s="92"/>
+      <c r="S30" s="91"/>
+      <c r="T30" s="91"/>
+      <c r="U30" s="91"/>
+      <c r="V30" s="91"/>
+      <c r="W30" s="91"/>
+      <c r="X30" s="91"/>
+      <c r="Y30" s="91"/>
+      <c r="Z30" s="91"/>
+      <c r="AA30" s="91"/>
+      <c r="AB30" s="91"/>
+      <c r="AC30" s="91"/>
+      <c r="AD30" s="91"/>
+      <c r="AE30" s="91"/>
+      <c r="AF30" s="91"/>
+      <c r="AG30" s="91"/>
+      <c r="AH30" s="91"/>
+      <c r="AI30" s="91"/>
+      <c r="AJ30" s="91"/>
+      <c r="AK30" s="91"/>
+      <c r="AL30" s="91"/>
+      <c r="AM30" s="91"/>
+      <c r="AN30" s="91"/>
+    </row>
+    <row r="31" spans="2:42" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="27"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-    </row>
-    <row r="32" spans="2:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="62" t="s">
+      <c r="C31" s="28"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="57"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="25"/>
+      <c r="W31" s="25"/>
+      <c r="X31" s="25"/>
+      <c r="Y31" s="25"/>
+      <c r="Z31" s="25"/>
+      <c r="AA31" s="25"/>
+      <c r="AB31" s="25"/>
+      <c r="AC31" s="25"/>
+      <c r="AD31" s="25"/>
+      <c r="AE31" s="25"/>
+      <c r="AF31" s="25"/>
+      <c r="AG31" s="25"/>
+      <c r="AH31" s="25"/>
+      <c r="AI31" s="25"/>
+      <c r="AJ31" s="25"/>
+      <c r="AK31" s="25"/>
+      <c r="AL31" s="25"/>
+      <c r="AM31" s="25"/>
+      <c r="AN31" s="25"/>
+    </row>
+    <row r="32" spans="2:42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="71" t="s">
+      <c r="D32" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="E32" s="57">
+      <c r="E32" s="53">
         <v>124</v>
       </c>
-      <c r="F32" s="52" t="s">
+      <c r="F32" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="G32" s="58">
+      <c r="G32" s="54">
         <v>214</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="35" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="58"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="22"/>
-      <c r="U35" s="22"/>
-    </row>
-    <row r="36" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="29"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="54"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="91"/>
+      <c r="S35" s="91"/>
+      <c r="T35" s="91"/>
+      <c r="U35" s="91"/>
+      <c r="V35" s="91"/>
+      <c r="W35" s="91"/>
+      <c r="X35" s="91"/>
+      <c r="Y35" s="91"/>
+      <c r="Z35" s="91"/>
+      <c r="AA35" s="91"/>
+      <c r="AB35" s="91"/>
+      <c r="AC35" s="91"/>
+      <c r="AD35" s="91"/>
+      <c r="AE35" s="91"/>
+      <c r="AF35" s="91"/>
+      <c r="AG35" s="91"/>
+      <c r="AH35" s="91"/>
+      <c r="AI35" s="91"/>
+      <c r="AJ35" s="91"/>
+      <c r="AK35" s="91"/>
+      <c r="AL35" s="91"/>
+      <c r="AM35" s="91"/>
+      <c r="AN35" s="91"/>
+    </row>
+    <row r="36" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="58"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="22"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="22"/>
-      <c r="U36" s="22"/>
-    </row>
-    <row r="37" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="62"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="22"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="54"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="91"/>
+      <c r="S36" s="91"/>
+      <c r="T36" s="91"/>
+      <c r="U36" s="91"/>
+      <c r="V36" s="91"/>
+      <c r="W36" s="91"/>
+      <c r="X36" s="91"/>
+      <c r="Y36" s="91"/>
+      <c r="Z36" s="91"/>
+      <c r="AA36" s="91"/>
+      <c r="AB36" s="91"/>
+      <c r="AC36" s="91"/>
+      <c r="AD36" s="91"/>
+      <c r="AE36" s="91"/>
+      <c r="AF36" s="91"/>
+      <c r="AG36" s="91"/>
+      <c r="AH36" s="91"/>
+      <c r="AI36" s="91"/>
+      <c r="AJ36" s="91"/>
+      <c r="AK36" s="91"/>
+      <c r="AL36" s="91"/>
+      <c r="AM36" s="91"/>
+      <c r="AN36" s="91"/>
+    </row>
+    <row r="37" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="58"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="20"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-      <c r="T37" s="22"/>
-      <c r="U37" s="22"/>
-    </row>
-    <row r="38" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="91"/>
+      <c r="S37" s="91"/>
+      <c r="T37" s="91"/>
+      <c r="U37" s="91"/>
+      <c r="V37" s="91"/>
+      <c r="W37" s="91"/>
+      <c r="X37" s="91"/>
+      <c r="Y37" s="91"/>
+      <c r="Z37" s="91"/>
+      <c r="AA37" s="91"/>
+      <c r="AB37" s="91"/>
+      <c r="AC37" s="91"/>
+      <c r="AD37" s="91"/>
+      <c r="AE37" s="91"/>
+      <c r="AF37" s="91"/>
+      <c r="AG37" s="91"/>
+      <c r="AH37" s="91"/>
+      <c r="AI37" s="91"/>
+      <c r="AJ37" s="91"/>
+      <c r="AK37" s="91"/>
+      <c r="AL37" s="91"/>
+      <c r="AM37" s="91"/>
+      <c r="AN37" s="91"/>
+    </row>
+    <row r="38" spans="2:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="73"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="61"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="27"/>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="27"/>
-    </row>
-    <row r="39" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="62" t="s">
+      <c r="C38" s="28"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="25"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="25"/>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="25"/>
+      <c r="S38" s="25"/>
+      <c r="T38" s="25"/>
+      <c r="U38" s="25"/>
+      <c r="V38" s="25"/>
+      <c r="W38" s="25"/>
+      <c r="X38" s="25"/>
+      <c r="Y38" s="25"/>
+      <c r="Z38" s="25"/>
+      <c r="AA38" s="25"/>
+      <c r="AB38" s="25"/>
+      <c r="AC38" s="25"/>
+      <c r="AD38" s="25"/>
+      <c r="AE38" s="25"/>
+      <c r="AF38" s="25"/>
+      <c r="AG38" s="25"/>
+      <c r="AH38" s="25"/>
+      <c r="AI38" s="25"/>
+      <c r="AJ38" s="25"/>
+      <c r="AK38" s="25"/>
+      <c r="AL38" s="25"/>
+      <c r="AM38" s="25"/>
+      <c r="AN38" s="25"/>
+    </row>
+    <row r="39" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="71" t="s">
+      <c r="D39" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="E39" s="57">
+      <c r="E39" s="53">
         <v>125</v>
       </c>
-      <c r="F39" s="52" t="s">
+      <c r="F39" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="G39" s="58">
+      <c r="G39" s="54">
         <v>215</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="11" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="11"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="22"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="20"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="22"/>
-    </row>
-    <row r="45" spans="2:21" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="91"/>
+      <c r="S44" s="91"/>
+      <c r="T44" s="91"/>
+      <c r="U44" s="91"/>
+      <c r="V44" s="91"/>
+      <c r="W44" s="91"/>
+      <c r="X44" s="91"/>
+      <c r="Y44" s="91"/>
+      <c r="Z44" s="91"/>
+      <c r="AA44" s="91"/>
+      <c r="AB44" s="91"/>
+      <c r="AC44" s="91"/>
+      <c r="AD44" s="91"/>
+      <c r="AE44" s="91"/>
+      <c r="AF44" s="91"/>
+      <c r="AG44" s="91"/>
+      <c r="AH44" s="91"/>
+      <c r="AI44" s="91"/>
+      <c r="AJ44" s="91"/>
+      <c r="AK44" s="91"/>
+      <c r="AL44" s="91"/>
+      <c r="AM44" s="91"/>
+      <c r="AN44" s="91"/>
+    </row>
+    <row r="45" spans="2:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C45" s="64" t="s">
+      <c r="C45" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="73" t="s">
+      <c r="D45" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="E45" s="59"/>
-      <c r="F45" s="60" t="s">
+      <c r="E45" s="55"/>
+      <c r="F45" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="G45" s="61">
+      <c r="G45" s="57">
         <v>233</v>
       </c>
-      <c r="H45" s="27">
+      <c r="H45" s="25">
         <v>8</v>
       </c>
-      <c r="I45" s="28" t="s">
+      <c r="I45" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="J45" s="27" t="s">
+      <c r="J45" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="K45" s="27" t="s">
+      <c r="K45" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="L45" s="27" t="s">
+      <c r="L45" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="M45" s="27" t="s">
+      <c r="M45" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="N45" s="27" t="s">
+      <c r="N45" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="O45" s="27" t="s">
+      <c r="O45" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="P45" s="27" t="s">
+      <c r="P45" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="Q45" s="27" t="s">
+      <c r="Q45" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27"/>
-      <c r="T45" s="27"/>
-      <c r="U45" s="27"/>
-    </row>
-    <row r="46" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R45" s="25"/>
+      <c r="S45" s="25"/>
+      <c r="T45" s="25"/>
+      <c r="U45" s="25"/>
+      <c r="V45" s="25"/>
+      <c r="W45" s="25"/>
+      <c r="X45" s="25"/>
+      <c r="Y45" s="25"/>
+      <c r="Z45" s="25"/>
+      <c r="AA45" s="25"/>
+      <c r="AB45" s="25"/>
+      <c r="AC45" s="25"/>
+      <c r="AD45" s="25"/>
+      <c r="AE45" s="25"/>
+      <c r="AF45" s="25"/>
+      <c r="AG45" s="25"/>
+      <c r="AH45" s="25"/>
+      <c r="AI45" s="25"/>
+      <c r="AJ45" s="25"/>
+      <c r="AK45" s="25"/>
+      <c r="AL45" s="25"/>
+      <c r="AM45" s="25"/>
+      <c r="AN45" s="25"/>
+    </row>
+    <row r="46" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="3"/>
-      <c r="C46" s="31"/>
-    </row>
-    <row r="47" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="29"/>
+    </row>
+    <row r="47" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C47" s="62" t="s">
+      <c r="C47" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="D47" s="71" t="s">
+      <c r="D47" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="F47" s="52" t="s">
+      <c r="F47" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="G47" s="53">
+      <c r="G47" s="49">
         <v>232</v>
       </c>
-      <c r="H47" s="22">
+      <c r="H47" s="20">
         <v>8</v>
       </c>
       <c r="I47" s="2" t="s">
@@ -2764,28 +3208,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C49" s="62" t="s">
+      <c r="C49" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="D49" s="71" t="s">
+      <c r="D49" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="F49" s="52" t="s">
+      <c r="F49" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="G49" s="53">
+      <c r="G49" s="49">
         <v>231</v>
       </c>
-      <c r="H49" s="22">
+      <c r="H49" s="20">
         <v>8</v>
       </c>
       <c r="I49" s="2" t="s">
@@ -2816,16 +3260,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C50" s="62"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="22"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="20"/>
       <c r="I50" s="2" t="s">
         <v>95</v>
       </c>
@@ -2849,111 +3293,149 @@
       </c>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
-      <c r="R50" s="22"/>
-      <c r="S50" s="22"/>
-      <c r="T50" s="22"/>
-      <c r="U50" s="22"/>
-    </row>
-    <row r="51" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R50" s="91"/>
+      <c r="S50" s="91"/>
+      <c r="T50" s="91"/>
+      <c r="U50" s="91"/>
+      <c r="V50" s="91"/>
+      <c r="W50" s="91"/>
+      <c r="X50" s="91"/>
+      <c r="Y50" s="91"/>
+      <c r="Z50" s="91"/>
+      <c r="AA50" s="91"/>
+      <c r="AB50" s="91"/>
+      <c r="AC50" s="91"/>
+      <c r="AD50" s="91"/>
+      <c r="AE50" s="91"/>
+      <c r="AF50" s="91"/>
+      <c r="AG50" s="91"/>
+      <c r="AH50" s="91"/>
+      <c r="AI50" s="91"/>
+      <c r="AJ50" s="91"/>
+      <c r="AK50" s="91"/>
+      <c r="AL50" s="91"/>
+      <c r="AM50" s="91"/>
+      <c r="AN50" s="91"/>
+    </row>
+    <row r="51" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="11"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="22"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="20"/>
       <c r="I51" s="2"/>
-      <c r="J51" s="22" t="s">
+      <c r="J51" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="K51" s="22" t="s">
+      <c r="K51" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="L51" s="22" t="s">
+      <c r="L51" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="M51" s="22" t="s">
+      <c r="M51" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="N51" s="22" t="s">
+      <c r="N51" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="O51" s="22" t="s">
+      <c r="O51" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="22"/>
-      <c r="T51" s="22"/>
-      <c r="U51" s="22"/>
-    </row>
-    <row r="52" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J52" s="22" t="s">
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="91"/>
+      <c r="S51" s="91"/>
+      <c r="T51" s="91"/>
+      <c r="U51" s="91"/>
+      <c r="V51" s="91"/>
+      <c r="W51" s="91"/>
+      <c r="X51" s="91"/>
+      <c r="Y51" s="91"/>
+      <c r="Z51" s="91"/>
+      <c r="AA51" s="91"/>
+      <c r="AB51" s="91"/>
+      <c r="AC51" s="91"/>
+      <c r="AD51" s="91"/>
+      <c r="AE51" s="91"/>
+      <c r="AF51" s="91"/>
+      <c r="AG51" s="91"/>
+      <c r="AH51" s="91"/>
+      <c r="AI51" s="91"/>
+      <c r="AJ51" s="91"/>
+      <c r="AK51" s="91"/>
+      <c r="AL51" s="91"/>
+      <c r="AM51" s="91"/>
+      <c r="AN51" s="91"/>
+    </row>
+    <row r="52" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J52" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="K52" s="22" t="s">
+      <c r="K52" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="L52" s="22" t="s">
+      <c r="L52" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="M52" s="22" t="s">
+      <c r="M52" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N52" s="22" t="s">
+      <c r="N52" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="O52" s="22" t="s">
+      <c r="O52" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="22"/>
-      <c r="O53" s="22"/>
-    </row>
-    <row r="54" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="62" t="s">
+    <row r="53" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="20"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="20"/>
+    </row>
+    <row r="54" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="71" t="s">
+      <c r="D54" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="E54" s="51">
+      <c r="E54" s="47">
         <v>122</v>
       </c>
-      <c r="F54" s="52" t="s">
+      <c r="F54" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="G54" s="53">
+      <c r="G54" s="49">
         <v>230</v>
       </c>
-      <c r="H54" s="22">
+      <c r="H54" s="20">
         <v>8</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="J54" s="22" t="s">
+      <c r="J54" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="K54" s="22" t="s">
+      <c r="K54" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="L54" s="22" t="s">
+      <c r="L54" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="M54" s="22" t="s">
+      <c r="M54" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="N54" s="22" t="s">
+      <c r="N54" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="O54" s="22" t="s">
+      <c r="O54" s="20" t="s">
         <v>67</v>
       </c>
       <c r="P54" s="1" t="s">
@@ -2963,426 +3445,605 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J55" s="22"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="22"/>
-      <c r="O55" s="22"/>
-    </row>
-    <row r="56" spans="2:21" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+    </row>
+    <row r="56" spans="2:40" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="10"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="60"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="27"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="27"/>
-      <c r="S56" s="27"/>
-      <c r="T56" s="27"/>
-      <c r="U56" s="27"/>
-    </row>
-    <row r="57" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="60"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="25"/>
+      <c r="K56" s="25"/>
+      <c r="L56" s="25"/>
+      <c r="M56" s="25"/>
+      <c r="N56" s="25"/>
+      <c r="O56" s="25"/>
+      <c r="P56" s="25"/>
+      <c r="Q56" s="25"/>
+      <c r="R56" s="25"/>
+      <c r="S56" s="25"/>
+      <c r="T56" s="25"/>
+      <c r="U56" s="25"/>
+      <c r="V56" s="25"/>
+      <c r="W56" s="25"/>
+      <c r="X56" s="25"/>
+      <c r="Y56" s="25"/>
+      <c r="Z56" s="25"/>
+      <c r="AA56" s="25"/>
+      <c r="AB56" s="25"/>
+      <c r="AC56" s="25"/>
+      <c r="AD56" s="25"/>
+      <c r="AE56" s="25"/>
+      <c r="AF56" s="25"/>
+      <c r="AG56" s="25"/>
+      <c r="AH56" s="25"/>
+      <c r="AI56" s="25"/>
+      <c r="AJ56" s="25"/>
+      <c r="AK56" s="25"/>
+      <c r="AL56" s="25"/>
+      <c r="AM56" s="25"/>
+      <c r="AN56" s="25"/>
+    </row>
+    <row r="57" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="11"/>
-      <c r="C57" s="62" t="s">
+      <c r="C57" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="D57" s="71">
+      <c r="D57" s="67">
         <v>77</v>
       </c>
-      <c r="E57" s="57">
+      <c r="E57" s="53">
         <v>119</v>
       </c>
-      <c r="F57" s="52" t="s">
+      <c r="F57" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="G57" s="58">
+      <c r="G57" s="54">
         <v>234</v>
       </c>
-      <c r="H57" s="22"/>
+      <c r="H57" s="20"/>
       <c r="I57" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J57" s="22" t="s">
+      <c r="J57" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="K57" s="22" t="s">
+      <c r="K57" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="L57" s="22" t="s">
+      <c r="L57" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="M57" s="22" t="s">
+      <c r="M57" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="N57" s="22" t="s">
+      <c r="N57" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="O57" s="22" t="s">
+      <c r="O57" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="P57" s="22" t="s">
+      <c r="P57" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="Q57" s="22" t="s">
+      <c r="Q57" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="S57" s="22"/>
-      <c r="T57" s="22"/>
-      <c r="U57" s="22"/>
-    </row>
-    <row r="58" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R57" s="91"/>
+      <c r="S57" s="91"/>
+      <c r="T57" s="91"/>
+      <c r="U57" s="91"/>
+      <c r="V57" s="91"/>
+      <c r="W57" s="91"/>
+      <c r="X57" s="91"/>
+      <c r="Y57" s="91"/>
+      <c r="Z57" s="91"/>
+      <c r="AA57" s="91"/>
+      <c r="AB57" s="91"/>
+      <c r="AC57" s="91"/>
+      <c r="AD57" s="91"/>
+      <c r="AE57" s="91"/>
+      <c r="AF57" s="91"/>
+      <c r="AG57" s="91"/>
+      <c r="AH57" s="91"/>
+      <c r="AI57" s="91"/>
+      <c r="AJ57" s="91"/>
+      <c r="AK57" s="91"/>
+      <c r="AL57" s="91"/>
+      <c r="AM57" s="91"/>
+      <c r="AN57" s="91"/>
+    </row>
+    <row r="58" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="11"/>
-      <c r="C58" s="62"/>
-      <c r="D58" s="71"/>
-      <c r="E58" s="57"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="22"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="67"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="20"/>
       <c r="I58" s="2"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22"/>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
-      <c r="S58" s="22"/>
-      <c r="T58" s="22"/>
-      <c r="U58" s="22"/>
-    </row>
-    <row r="59" spans="2:21" s="86" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="87"/>
-      <c r="C59" s="88"/>
-      <c r="D59" s="89"/>
-      <c r="E59" s="90"/>
-      <c r="F59" s="91"/>
-      <c r="G59" s="81"/>
-      <c r="H59" s="92"/>
-      <c r="I59" s="93"/>
-      <c r="J59" s="92"/>
-      <c r="K59" s="92"/>
-      <c r="L59" s="92"/>
-      <c r="M59" s="92"/>
-      <c r="N59" s="92"/>
-      <c r="O59" s="92"/>
-      <c r="P59" s="92"/>
-      <c r="Q59" s="92"/>
-      <c r="R59" s="92"/>
-      <c r="S59" s="92"/>
-      <c r="T59" s="92"/>
-      <c r="U59" s="92"/>
-    </row>
-    <row r="60" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="91"/>
+      <c r="S58" s="91"/>
+      <c r="T58" s="91"/>
+      <c r="U58" s="91"/>
+      <c r="V58" s="91"/>
+      <c r="W58" s="91"/>
+      <c r="X58" s="91"/>
+      <c r="Y58" s="91"/>
+      <c r="Z58" s="91"/>
+      <c r="AA58" s="91"/>
+      <c r="AB58" s="91"/>
+      <c r="AC58" s="91"/>
+      <c r="AD58" s="91"/>
+      <c r="AE58" s="91"/>
+      <c r="AF58" s="91"/>
+      <c r="AG58" s="91"/>
+      <c r="AH58" s="91"/>
+      <c r="AI58" s="91"/>
+      <c r="AJ58" s="91"/>
+      <c r="AK58" s="91"/>
+      <c r="AL58" s="91"/>
+      <c r="AM58" s="91"/>
+      <c r="AN58" s="91"/>
+    </row>
+    <row r="59" spans="2:40" s="82" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="83"/>
+      <c r="C59" s="84"/>
+      <c r="D59" s="85"/>
+      <c r="E59" s="86"/>
+      <c r="F59" s="87"/>
+      <c r="G59" s="77"/>
+      <c r="H59" s="88"/>
+      <c r="I59" s="89"/>
+      <c r="J59" s="88"/>
+      <c r="K59" s="88"/>
+      <c r="L59" s="88"/>
+      <c r="M59" s="88"/>
+      <c r="N59" s="88"/>
+      <c r="O59" s="88"/>
+      <c r="P59" s="88"/>
+      <c r="Q59" s="88"/>
+      <c r="R59" s="88"/>
+      <c r="S59" s="88"/>
+      <c r="T59" s="88"/>
+      <c r="U59" s="88"/>
+      <c r="V59" s="88"/>
+      <c r="W59" s="88"/>
+      <c r="X59" s="88"/>
+      <c r="Y59" s="88"/>
+      <c r="Z59" s="88"/>
+      <c r="AA59" s="88"/>
+      <c r="AB59" s="88"/>
+      <c r="AC59" s="88"/>
+      <c r="AD59" s="88"/>
+      <c r="AE59" s="88"/>
+      <c r="AF59" s="88"/>
+      <c r="AG59" s="88"/>
+      <c r="AH59" s="88"/>
+      <c r="AI59" s="88"/>
+      <c r="AJ59" s="88"/>
+      <c r="AK59" s="88"/>
+      <c r="AL59" s="88"/>
+      <c r="AM59" s="88"/>
+      <c r="AN59" s="88"/>
+    </row>
+    <row r="60" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="11"/>
-      <c r="C60" s="62"/>
-      <c r="D60" s="71"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="52"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="74"/>
-      <c r="I60" s="75"/>
-      <c r="J60" s="74"/>
-      <c r="K60" s="74"/>
-      <c r="L60" s="74"/>
-      <c r="M60" s="74"/>
-      <c r="N60" s="74"/>
-      <c r="O60" s="74"/>
-      <c r="P60" s="74"/>
-      <c r="Q60" s="74"/>
-      <c r="R60" s="74"/>
-      <c r="S60" s="74"/>
-      <c r="T60" s="74"/>
-      <c r="U60" s="74"/>
-    </row>
-    <row r="61" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="94" t="s">
+      <c r="C60" s="58"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="71"/>
+      <c r="J60" s="70"/>
+      <c r="K60" s="70"/>
+      <c r="L60" s="70"/>
+      <c r="M60" s="70"/>
+      <c r="N60" s="70"/>
+      <c r="O60" s="70"/>
+      <c r="P60" s="70"/>
+      <c r="Q60" s="70"/>
+      <c r="R60" s="91"/>
+      <c r="S60" s="91"/>
+      <c r="T60" s="91"/>
+      <c r="U60" s="91"/>
+      <c r="V60" s="91"/>
+      <c r="W60" s="91"/>
+      <c r="X60" s="91"/>
+      <c r="Y60" s="91"/>
+      <c r="Z60" s="91"/>
+      <c r="AA60" s="91"/>
+      <c r="AB60" s="91"/>
+      <c r="AC60" s="91"/>
+      <c r="AD60" s="91"/>
+      <c r="AE60" s="91"/>
+      <c r="AF60" s="91"/>
+      <c r="AG60" s="91"/>
+      <c r="AH60" s="91"/>
+      <c r="AI60" s="91"/>
+      <c r="AJ60" s="91"/>
+      <c r="AK60" s="91"/>
+      <c r="AL60" s="91"/>
+      <c r="AM60" s="91"/>
+      <c r="AN60" s="91"/>
+    </row>
+    <row r="61" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="C61" s="62" t="s">
+      <c r="C61" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="D61" s="71" t="s">
+      <c r="D61" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E61" s="57"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="58">
+      <c r="E61" s="53"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="54">
         <v>200</v>
       </c>
-      <c r="H61" s="74">
+      <c r="H61" s="70">
         <v>3</v>
       </c>
-      <c r="I61" s="75" t="s">
+      <c r="I61" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="J61" s="74">
+      <c r="J61" s="70">
         <v>0</v>
       </c>
-      <c r="K61" s="74">
+      <c r="K61" s="70">
         <v>0</v>
       </c>
-      <c r="L61" s="74" t="s">
+      <c r="L61" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="M61" s="74"/>
-      <c r="N61" s="74"/>
-      <c r="O61" s="74"/>
-      <c r="P61" s="74"/>
-      <c r="Q61" s="74"/>
-      <c r="R61" s="74"/>
-      <c r="S61" s="74"/>
-      <c r="T61" s="74"/>
-      <c r="U61" s="74"/>
-    </row>
-    <row r="62" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M61" s="70"/>
+      <c r="N61" s="70"/>
+      <c r="O61" s="70"/>
+      <c r="P61" s="70"/>
+      <c r="Q61" s="70"/>
+      <c r="R61" s="91"/>
+      <c r="S61" s="91"/>
+      <c r="T61" s="91"/>
+      <c r="U61" s="91"/>
+      <c r="V61" s="91"/>
+      <c r="W61" s="91"/>
+      <c r="X61" s="91"/>
+      <c r="Y61" s="91"/>
+      <c r="Z61" s="91"/>
+      <c r="AA61" s="91"/>
+      <c r="AB61" s="91"/>
+      <c r="AC61" s="91"/>
+      <c r="AD61" s="91"/>
+      <c r="AE61" s="91"/>
+      <c r="AF61" s="91"/>
+      <c r="AG61" s="91"/>
+      <c r="AH61" s="91"/>
+      <c r="AI61" s="91"/>
+      <c r="AJ61" s="91"/>
+      <c r="AK61" s="91"/>
+      <c r="AL61" s="91"/>
+      <c r="AM61" s="91"/>
+      <c r="AN61" s="91"/>
+    </row>
+    <row r="62" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="11"/>
-      <c r="C62" s="62"/>
-      <c r="D62" s="71"/>
-      <c r="E62" s="57"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="74"/>
-      <c r="I62" s="75"/>
-      <c r="J62" s="74"/>
-      <c r="K62" s="74"/>
-      <c r="L62" s="74"/>
-      <c r="M62" s="74"/>
-      <c r="N62" s="74"/>
-      <c r="O62" s="74"/>
-      <c r="P62" s="74"/>
-      <c r="Q62" s="74"/>
-      <c r="R62" s="74"/>
-      <c r="S62" s="74"/>
-      <c r="T62" s="74"/>
-      <c r="U62" s="74"/>
-    </row>
-    <row r="63" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="58"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="54"/>
+      <c r="H62" s="70"/>
+      <c r="I62" s="71"/>
+      <c r="J62" s="70"/>
+      <c r="K62" s="70"/>
+      <c r="L62" s="70"/>
+      <c r="M62" s="70"/>
+      <c r="N62" s="70"/>
+      <c r="O62" s="70"/>
+      <c r="P62" s="70"/>
+      <c r="Q62" s="70"/>
+      <c r="R62" s="91"/>
+      <c r="S62" s="91"/>
+      <c r="T62" s="91"/>
+      <c r="U62" s="91"/>
+      <c r="V62" s="91"/>
+      <c r="W62" s="91"/>
+      <c r="X62" s="91"/>
+      <c r="Y62" s="91"/>
+      <c r="Z62" s="91"/>
+      <c r="AA62" s="91"/>
+      <c r="AB62" s="91"/>
+      <c r="AC62" s="91"/>
+      <c r="AD62" s="91"/>
+      <c r="AE62" s="91"/>
+      <c r="AF62" s="91"/>
+      <c r="AG62" s="91"/>
+      <c r="AH62" s="91"/>
+      <c r="AI62" s="91"/>
+      <c r="AJ62" s="91"/>
+      <c r="AK62" s="91"/>
+      <c r="AL62" s="91"/>
+      <c r="AM62" s="91"/>
+      <c r="AN62" s="91"/>
+    </row>
+    <row r="63" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="11"/>
-      <c r="C63" s="62" t="s">
+      <c r="C63" s="58" t="s">
         <v>174</v>
       </c>
-      <c r="D63" s="71" t="s">
+      <c r="D63" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E63" s="57"/>
-      <c r="F63" s="52"/>
-      <c r="G63" s="58">
+      <c r="E63" s="53"/>
+      <c r="F63" s="48"/>
+      <c r="G63" s="54">
         <v>201</v>
       </c>
-      <c r="H63" s="74">
+      <c r="H63" s="70">
         <v>5</v>
       </c>
-      <c r="I63" s="75">
+      <c r="I63" s="71">
         <v>201</v>
       </c>
-      <c r="J63" s="74">
+      <c r="J63" s="70">
         <v>201</v>
       </c>
-      <c r="K63" s="74" t="s">
+      <c r="K63" s="70" t="s">
         <v>175</v>
       </c>
-      <c r="L63" s="74" t="s">
+      <c r="L63" s="70" t="s">
         <v>176</v>
       </c>
-      <c r="M63" s="74" t="s">
+      <c r="M63" s="70" t="s">
         <v>177</v>
       </c>
-      <c r="N63" s="74" t="s">
+      <c r="N63" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="O63" s="74"/>
-      <c r="P63" s="74"/>
-      <c r="Q63" s="74"/>
-      <c r="R63" s="74"/>
-      <c r="S63" s="74"/>
-      <c r="T63" s="74"/>
-      <c r="U63" s="74"/>
-    </row>
-    <row r="64" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O63" s="70"/>
+      <c r="P63" s="70"/>
+      <c r="Q63" s="70"/>
+      <c r="R63" s="91"/>
+      <c r="S63" s="91"/>
+      <c r="T63" s="91"/>
+      <c r="U63" s="91"/>
+      <c r="V63" s="91"/>
+      <c r="W63" s="91"/>
+      <c r="X63" s="91"/>
+      <c r="Y63" s="91"/>
+      <c r="Z63" s="91"/>
+      <c r="AA63" s="91"/>
+      <c r="AB63" s="91"/>
+      <c r="AC63" s="91"/>
+      <c r="AD63" s="91"/>
+      <c r="AE63" s="91"/>
+      <c r="AF63" s="91"/>
+      <c r="AG63" s="91"/>
+      <c r="AH63" s="91"/>
+      <c r="AI63" s="91"/>
+      <c r="AJ63" s="91"/>
+      <c r="AK63" s="91"/>
+      <c r="AL63" s="91"/>
+      <c r="AM63" s="91"/>
+      <c r="AN63" s="91"/>
+    </row>
+    <row r="64" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="11"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="71"/>
-      <c r="E64" s="57"/>
-      <c r="F64" s="52"/>
-      <c r="G64" s="58"/>
-      <c r="H64" s="74"/>
-      <c r="I64" s="75"/>
-      <c r="J64" s="74"/>
-      <c r="K64" s="74"/>
-      <c r="L64" s="74"/>
-      <c r="M64" s="74"/>
-      <c r="N64" s="74"/>
-      <c r="O64" s="74"/>
-      <c r="P64" s="74"/>
-      <c r="Q64" s="74"/>
-      <c r="R64" s="74"/>
-      <c r="S64" s="74"/>
-      <c r="T64" s="74"/>
-      <c r="U64" s="74"/>
-    </row>
-    <row r="65" spans="2:21" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="58"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="54"/>
+      <c r="H64" s="70"/>
+      <c r="I64" s="71"/>
+      <c r="J64" s="70"/>
+      <c r="K64" s="70"/>
+      <c r="L64" s="70"/>
+      <c r="M64" s="70"/>
+      <c r="N64" s="70"/>
+      <c r="O64" s="70"/>
+      <c r="P64" s="70"/>
+      <c r="Q64" s="70"/>
+      <c r="R64" s="91"/>
+      <c r="S64" s="91"/>
+      <c r="T64" s="91"/>
+      <c r="U64" s="91"/>
+      <c r="V64" s="91"/>
+      <c r="W64" s="91"/>
+      <c r="X64" s="91"/>
+      <c r="Y64" s="91"/>
+      <c r="Z64" s="91"/>
+      <c r="AA64" s="91"/>
+      <c r="AB64" s="91"/>
+      <c r="AC64" s="91"/>
+      <c r="AD64" s="91"/>
+      <c r="AE64" s="91"/>
+      <c r="AF64" s="91"/>
+      <c r="AG64" s="91"/>
+      <c r="AH64" s="91"/>
+      <c r="AI64" s="91"/>
+      <c r="AJ64" s="91"/>
+      <c r="AK64" s="91"/>
+      <c r="AL64" s="91"/>
+      <c r="AM64" s="91"/>
+      <c r="AN64" s="91"/>
+    </row>
+    <row r="65" spans="2:40" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="11"/>
-      <c r="C65" s="62"/>
-      <c r="D65" s="71"/>
-      <c r="E65" s="57"/>
-      <c r="F65" s="52"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="74"/>
-      <c r="I65" s="75"/>
-      <c r="J65" s="74"/>
-      <c r="K65" s="74"/>
-      <c r="L65" s="74"/>
-      <c r="M65" s="74"/>
-      <c r="N65" s="74"/>
-      <c r="O65" s="74"/>
-      <c r="P65" s="74"/>
-      <c r="Q65" s="74"/>
-      <c r="R65" s="74"/>
-      <c r="S65" s="74"/>
-      <c r="T65" s="74"/>
-      <c r="U65" s="74"/>
-    </row>
-    <row r="66" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="82" t="s">
+      <c r="C65" s="58"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="54"/>
+      <c r="H65" s="70"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="70"/>
+      <c r="K65" s="70"/>
+      <c r="L65" s="70"/>
+      <c r="M65" s="70"/>
+      <c r="N65" s="70"/>
+      <c r="O65" s="70"/>
+      <c r="P65" s="70"/>
+      <c r="Q65" s="70"/>
+      <c r="R65" s="91"/>
+      <c r="S65" s="91"/>
+      <c r="T65" s="91"/>
+      <c r="U65" s="91"/>
+      <c r="V65" s="91"/>
+      <c r="W65" s="91"/>
+      <c r="X65" s="91"/>
+      <c r="Y65" s="91"/>
+      <c r="Z65" s="91"/>
+      <c r="AA65" s="91"/>
+      <c r="AB65" s="91"/>
+      <c r="AC65" s="91"/>
+      <c r="AD65" s="91"/>
+      <c r="AE65" s="91"/>
+      <c r="AF65" s="91"/>
+      <c r="AG65" s="91"/>
+      <c r="AH65" s="91"/>
+      <c r="AI65" s="91"/>
+      <c r="AJ65" s="91"/>
+      <c r="AK65" s="91"/>
+      <c r="AL65" s="91"/>
+      <c r="AM65" s="91"/>
+      <c r="AN65" s="91"/>
+    </row>
+    <row r="66" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="2:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="78" t="s">
         <v>170</v>
       </c>
-      <c r="D67" s="78" t="s">
+      <c r="D67" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="E67" s="79"/>
-      <c r="F67" s="80" t="s">
+      <c r="E67" s="75"/>
+      <c r="F67" s="76" t="s">
         <v>168</v>
       </c>
-      <c r="G67" s="81"/>
-    </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B68" s="77" t="s">
+      <c r="G67" s="77"/>
+    </row>
+    <row r="68" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B68" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="C68" s="76" t="s">
+      <c r="C68" s="72" t="s">
         <v>165</v>
       </c>
-      <c r="D68" s="71">
+      <c r="D68" s="67">
         <v>254</v>
       </c>
-      <c r="E68" s="51" t="s">
+      <c r="E68" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="52">
+      <c r="F68" s="48">
         <v>253</v>
       </c>
-      <c r="G68" s="53" t="s">
+      <c r="G68" s="49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B69" s="77"/>
-      <c r="C69" s="76"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="29"/>
-      <c r="J69" s="23"/>
-      <c r="K69" s="23"/>
-      <c r="L69" s="23"/>
-      <c r="M69" s="23"/>
-      <c r="N69" s="23"/>
-      <c r="O69" s="23"/>
-      <c r="P69" s="23"/>
-      <c r="Q69" s="23"/>
-      <c r="R69" s="23"/>
-      <c r="S69" s="23"/>
-      <c r="T69" s="23"/>
-      <c r="U69" s="23"/>
-    </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B70" s="77" t="s">
+    <row r="69" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B69" s="73"/>
+      <c r="C69" s="72"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="21"/>
+      <c r="N69" s="21"/>
+      <c r="O69" s="21"/>
+      <c r="P69" s="21"/>
+      <c r="Q69" s="21"/>
+    </row>
+    <row r="70" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B70" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="76" t="s">
+      <c r="C70" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="D70" s="71">
+      <c r="D70" s="67">
         <v>239</v>
       </c>
-      <c r="E70" s="51" t="s">
+      <c r="E70" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="F70" s="52">
+      <c r="F70" s="48">
         <v>237</v>
       </c>
-      <c r="G70" s="53" t="s">
+      <c r="G70" s="49" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B71" s="77"/>
-      <c r="C71" s="76"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="29"/>
-      <c r="J71" s="23"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="23"/>
-      <c r="M71" s="23"/>
-      <c r="N71" s="23"/>
-      <c r="O71" s="23"/>
-      <c r="P71" s="23"/>
-      <c r="Q71" s="23"/>
-      <c r="R71" s="23"/>
-      <c r="S71" s="23"/>
-      <c r="T71" s="23"/>
-      <c r="U71" s="23"/>
-    </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B72" s="77" t="s">
+    <row r="71" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B71" s="73"/>
+      <c r="C71" s="72"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="27"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="21"/>
+      <c r="M71" s="21"/>
+      <c r="N71" s="21"/>
+      <c r="O71" s="21"/>
+      <c r="P71" s="21"/>
+      <c r="Q71" s="21"/>
+    </row>
+    <row r="72" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B72" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C72" s="76" t="s">
+      <c r="C72" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="F72" s="52">
+      <c r="F72" s="48">
         <v>211</v>
       </c>
-      <c r="G72" s="53" t="s">
+      <c r="G72" s="49" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B73" s="77"/>
-      <c r="C73" s="76"/>
-      <c r="H73" s="24"/>
-      <c r="I73" s="29"/>
-      <c r="J73" s="23"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="23"/>
-      <c r="M73" s="23"/>
-      <c r="N73" s="23"/>
-      <c r="O73" s="23"/>
-      <c r="P73" s="23"/>
-      <c r="Q73" s="23"/>
-      <c r="R73" s="23"/>
-      <c r="S73" s="23"/>
-      <c r="T73" s="23"/>
-      <c r="U73" s="23"/>
-    </row>
-    <row r="74" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B74" s="77" t="s">
+    <row r="73" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B73" s="73"/>
+      <c r="C73" s="72"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="27"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
+      <c r="M73" s="21"/>
+      <c r="N73" s="21"/>
+      <c r="O73" s="21"/>
+      <c r="P73" s="21"/>
+      <c r="Q73" s="21"/>
+    </row>
+    <row r="74" spans="2:40" x14ac:dyDescent="0.2">
+      <c r="B74" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="C74" s="76" t="s">
+      <c r="C74" s="72" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3404,12 +4065,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3577,15 +4235,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3609,17 +4278,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>